<commit_message>
Add pico quantification data
</commit_message>
<xml_diff>
--- a/data/fractionation/230329 Batch 143 Water Yr Summary.xlsx
+++ b/data/fractionation/230329 Batch 143 Water Yr Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Banfield\WaterYear\SIP\data\fractionation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F571A79E-B071-4F33-8364-E953BE7C59C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFFAEDE-7ABB-40E4-BCF9-C2F4930403FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <sheet name="Tube P" sheetId="19" r:id="rId19"/>
     <sheet name="time" sheetId="1" r:id="rId20"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId21"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -52,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="215">
   <si>
     <t>calculated density p(20)</t>
   </si>
@@ -681,12 +678,6 @@
   </si>
   <si>
     <t>DNA (ng/ul)</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>G</t>
@@ -2296,132 +2287,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$O$5:$O$23</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1.7626274340000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.758256394</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7527925940000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7464272670000014</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7398707070000015</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7354996669999991</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7291343399999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7225777799999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7171139799999988</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7105574199999989</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7050936199999995</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6996298200000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6932644929999991</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6878006929999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.683429653000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6779658530000017</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.671409293</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6473685729999996</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.5503041660000001</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Summary!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$P$5:$P$23</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-5.3538839960976458E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0608585303546176E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.10043130380465427</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.175360529597648</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.51863065556540644</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2204466196133288</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.9027148760908119</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0237378781819473</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.613331556357783</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.4605341772915512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.3960084085803111</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.581010398673115</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3562277425787963</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.83852948806109751</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.52749612099034315</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.27668119896078913</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.17970421821209173</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.17085276786947276</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.11322053679330339</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2465,132 +2341,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$R$5:$R$23</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1.7581197989999993</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7548415189999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7493777189999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7439139190000006</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7373573589999989</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7318935589999995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7255282320000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7200644320000009</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7146006319999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7102295919999992</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7047657919999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6982092320000017</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6918439049999989</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6863801049999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6798235450000014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6754525050000009</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6678031850000004</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6483247379999995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.5456052980000017</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Summary!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$S$5:$S$23</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.3851345744681399E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6906363608471935E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.22550491251158367</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.70629344241902603</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6691083790296721</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.6870802157983049</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.2523410638667016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16.462006311442085</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.7283074693526</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.907065732067259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.8807231378408487</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.1848577497107544</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6301457107211246</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.91438975316711246</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.63684669774874458</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.38816203621431278</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.30424702451426316</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.33403759007293782</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.24513757490331053</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2640,7 +2401,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$U$5:$U$23</c:f>
+              <c:f>Summary!$O$5:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2706,7 +2467,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$V$5:$V$23</c:f>
+              <c:f>Summary!$P$5:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2815,7 +2576,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$X$5:$X$23</c:f>
+              <c:f>Summary!$R$5:$R$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2881,7 +2642,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$Y$5:$Y$23</c:f>
+              <c:f>Summary!$S$5:$S$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -4215,75 +3976,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$O$4:$O$25</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7626274340000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7626274340000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.758256394</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7527925940000006</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7464272670000014</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7398707070000015</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7354996669999991</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7291343399999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7225777799999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7171139799999988</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7105574199999989</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7050936199999995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6996298200000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6932644929999991</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6878006929999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.683429653000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6779658530000017</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.671409293</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.6473685729999996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.5503041660000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.3339376860000005</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1066436060000004</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4402,75 +4100,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$R$4:$R$25</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7557430459999992</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7581197989999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7548415189999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7493777189999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7439139190000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7373573589999989</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.7318935589999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7255282320000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7200644320000009</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7146006319999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.7102295919999992</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7047657919999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6982092320000017</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6918439049999989</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6863801049999996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6798235450000014</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6754525050000009</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6678031850000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.6483247379999995</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.5456052980000017</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.3270532980000009</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1106868180000014</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4595,7 +4230,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$U$4:$U$25</c:f>
+              <c:f>Summary!$O$4:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -4788,7 +4423,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$X$4:$X$25</c:f>
+              <c:f>Summary!$R$4:$R$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -5756,7 +5391,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AA$4:$AA$25</c:f>
+              <c:f>Summary!$U$4:$U$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -5952,7 +5587,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AD$4:$AD$25</c:f>
+              <c:f>Summary!$X$4:$X$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -6148,7 +5783,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AG$4:$AG$25</c:f>
+              <c:f>Summary!$AA$4:$AA$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -6344,7 +5979,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AJ$4:$AJ$25</c:f>
+              <c:f>Summary!$AD$4:$AD$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -7130,7 +6765,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AA$5:$AA$23</c:f>
+              <c:f>Summary!$U$5:$U$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7196,7 +6831,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AB$5:$AB$23</c:f>
+              <c:f>Summary!$V$5:$V$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7308,7 +6943,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AD$5:$AD$23</c:f>
+              <c:f>Summary!$X$5:$X$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7374,7 +7009,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AE$5:$AE$23</c:f>
+              <c:f>Summary!$Y$5:$Y$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7486,7 +7121,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AG$5:$AG$23</c:f>
+              <c:f>Summary!$AA$5:$AA$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7552,7 +7187,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AH$5:$AH$23</c:f>
+              <c:f>Summary!$AB$5:$AB$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7664,7 +7299,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AJ$5:$AJ$23</c:f>
+              <c:f>Summary!$AD$5:$AD$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7730,7 +7365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AK$5:$AK$23</c:f>
+              <c:f>Summary!$AE$5:$AE$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -9850,8 +9485,8 @@
       <xdr:rowOff>61079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>277436</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>93134</xdr:rowOff>
     </xdr:to>
@@ -9880,13 +9515,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>3983</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>45572</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>484466</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>111186</xdr:rowOff>
@@ -9996,237 +9631,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Table of Contents"/>
-      <sheetName val="Summary"/>
-      <sheetName val="TubeLoading"/>
-      <sheetName val="Tube A"/>
-      <sheetName val="Tube B"/>
-      <sheetName val="Tube C"/>
-      <sheetName val="Tube D"/>
-      <sheetName val="Tube E"/>
-      <sheetName val="Tube F"/>
-      <sheetName val="Tube G"/>
-      <sheetName val="Tube H"/>
-      <sheetName val="Tube I"/>
-      <sheetName val="Tube J"/>
-      <sheetName val="Tube K"/>
-      <sheetName val="Tube L"/>
-      <sheetName val="Tube M"/>
-      <sheetName val="Tube N"/>
-      <sheetName val="Tube O"/>
-      <sheetName val="Tube P"/>
-      <sheetName val="time"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="C4">
-            <v>1.7708231340000022</v>
-          </cell>
-          <cell r="D4">
-            <v>-1.1510114882384404E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>1.7686376140000011</v>
-          </cell>
-          <cell r="D5">
-            <v>9.4157495119879392E-3</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>1.7653593340000029</v>
-          </cell>
-          <cell r="D6">
-            <v>2.0551110856287979E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>1.7609882940000006</v>
-          </cell>
-          <cell r="D7">
-            <v>2.2611151276471095E-2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>1.756617254</v>
-          </cell>
-          <cell r="D8">
-            <v>9.8983388727655174E-3</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>1.7522462140000012</v>
-          </cell>
-          <cell r="D9">
-            <v>4.5531010194395073E-2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>1.7478751740000007</v>
-          </cell>
-          <cell r="D10">
-            <v>7.6573787645410632E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>1.7435041340000019</v>
-          </cell>
-          <cell r="D11">
-            <v>8.4424705083593052E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>1.741318613999999</v>
-          </cell>
-          <cell r="D12">
-            <v>0.16372701548733104</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>1.7358548139999996</v>
-          </cell>
-          <cell r="D13">
-            <v>0.52404113188743595</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>1.7325765340000014</v>
-          </cell>
-          <cell r="D14">
-            <v>1.1617199169874437</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>1.7294894870000004</v>
-          </cell>
-          <cell r="D15">
-            <v>3.8310789256687445</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>1.7251184470000016</v>
-          </cell>
-          <cell r="D16">
-            <v>11.460547155457862</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>1.7218401670000016</v>
-          </cell>
-          <cell r="D17">
-            <v>19.354246927651218</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>1.7187531200000006</v>
-          </cell>
-          <cell r="D18">
-            <v>18.494310020815934</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>1.7154748400000006</v>
-          </cell>
-          <cell r="D19">
-            <v>16.556998700026551</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>1.7132893200000012</v>
-          </cell>
-          <cell r="D20">
-            <v>10.63528126752014</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>1.7078255200000019</v>
-          </cell>
-          <cell r="D21">
-            <v>7.9585961168425099</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>1.7045472400000019</v>
-          </cell>
-          <cell r="D22">
-            <v>3.7854063895958348</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>1.7012689600000019</v>
-          </cell>
-          <cell r="D23">
-            <v>1.9930382668107891</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>1.6979906800000002</v>
-          </cell>
-          <cell r="D24">
-            <v>1.4481880089780008</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>1.6936196399999996</v>
-          </cell>
-          <cell r="D25">
-            <v>1.2704311701056521</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10551,10 +9955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E138FBF1-D534-4F7E-950C-764D2E6B8C19}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A9" activeCellId="1" sqref="A10:XFD10 A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45"/>
@@ -10572,44 +9976,44 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>195</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -10622,7 +10026,7 @@
         <v>Tube A</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D5" s="67">
         <v>45014</v>
@@ -10631,7 +10035,7 @@
         <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G5" s="66">
         <f>TubeLoading!J29</f>
@@ -10645,7 +10049,7 @@
         <v>37</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10658,7 +10062,7 @@
         <v>Tube B</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="67">
         <v>45014</v>
@@ -10667,7 +10071,7 @@
         <v>112</v>
       </c>
       <c r="F6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G6" s="66">
         <f>TubeLoading!J30</f>
@@ -10691,7 +10095,7 @@
         <v>Tube C</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" s="67">
         <v>45014</v>
@@ -10700,7 +10104,7 @@
         <v>112</v>
       </c>
       <c r="F7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G7" s="66">
         <f>TubeLoading!J31</f>
@@ -10724,7 +10128,7 @@
         <v>Tube D</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D8" s="67">
         <v>45014</v>
@@ -10733,7 +10137,7 @@
         <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G8" s="66">
         <f>TubeLoading!J32</f>
@@ -10749,15 +10153,15 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="66">
-        <f>TubeLoading!F33</f>
-        <v>3193</v>
+        <f>TubeLoading!F35</f>
+        <v>3654</v>
       </c>
       <c r="B9" s="66" t="str">
-        <f>TubeLoading!A33</f>
-        <v>Tube E</v>
+        <f>TubeLoading!A35</f>
+        <v>Tube G</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D9" s="67">
         <v>45014</v>
@@ -10766,15 +10170,15 @@
         <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G9" s="66">
-        <f>TubeLoading!J33</f>
+        <f>TubeLoading!J35</f>
         <v>4000</v>
       </c>
       <c r="H9" s="50">
         <f>Summary!P26</f>
-        <v>44.543408475176868</v>
+        <v>64.286969553839086</v>
       </c>
       <c r="I9" s="114">
         <v>37</v>
@@ -10782,15 +10186,15 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="66">
-        <f>TubeLoading!F34</f>
-        <v>2383</v>
+        <f>TubeLoading!F36</f>
+        <v>1794</v>
       </c>
       <c r="B10" s="66" t="str">
-        <f>TubeLoading!A34</f>
-        <v>Tube F</v>
+        <f>TubeLoading!A36</f>
+        <v>Tube H</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D10" s="67">
         <v>45014</v>
@@ -10799,15 +10203,15 @@
         <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G10" s="66">
-        <f>TubeLoading!J34</f>
+        <f>TubeLoading!J36</f>
         <v>4000</v>
       </c>
       <c r="H10" s="50">
         <f>Summary!S26</f>
-        <v>75.593595322285182</v>
+        <v>73.330591175662391</v>
       </c>
       <c r="I10" s="115">
         <v>37</v>
@@ -10815,32 +10219,32 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="66">
-        <f>TubeLoading!F35</f>
-        <v>3654</v>
+        <f>TubeLoading!F41</f>
+        <v>4016</v>
       </c>
       <c r="B11" s="66" t="str">
-        <f>TubeLoading!A35</f>
-        <v>Tube G</v>
+        <f>TubeLoading!A41</f>
+        <v>Tube M</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D11" s="67">
         <v>45014</v>
       </c>
       <c r="E11">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="F11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G11" s="66">
-        <f>TubeLoading!J35</f>
-        <v>4000</v>
+        <f>TubeLoading!J41</f>
+        <v>3999.9999999999995</v>
       </c>
       <c r="H11" s="50">
         <f>Summary!V26</f>
-        <v>64.286969553839086</v>
+        <v>80.45097095349729</v>
       </c>
       <c r="I11" s="114">
         <v>37</v>
@@ -10848,32 +10252,32 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="66">
-        <f>TubeLoading!F36</f>
-        <v>1794</v>
+        <f>TubeLoading!F42</f>
+        <v>2445</v>
       </c>
       <c r="B12" s="66" t="str">
-        <f>TubeLoading!A36</f>
-        <v>Tube H</v>
+        <f>TubeLoading!A42</f>
+        <v>Tube N</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D12" s="67">
         <v>45014</v>
       </c>
       <c r="E12">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="F12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G12" s="66">
-        <f>TubeLoading!J36</f>
+        <f>TubeLoading!J42</f>
         <v>4000</v>
       </c>
       <c r="H12" s="50">
         <f>Summary!Y26</f>
-        <v>73.330591175662391</v>
+        <v>73.835192341047971</v>
       </c>
       <c r="I12" s="115">
         <v>37</v>
@@ -10881,15 +10285,15 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="66">
-        <f>TubeLoading!F41</f>
-        <v>4016</v>
+        <f>TubeLoading!F43</f>
+        <v>2021</v>
       </c>
       <c r="B13" s="66" t="str">
-        <f>TubeLoading!A41</f>
-        <v>Tube M</v>
+        <f>TubeLoading!A43</f>
+        <v>Tube O</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D13" s="67">
         <v>45014</v>
@@ -10898,31 +10302,34 @@
         <v>140</v>
       </c>
       <c r="F13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G13" s="66">
-        <f>TubeLoading!J41</f>
+        <f>TubeLoading!J43</f>
         <v>3999.9999999999995</v>
       </c>
       <c r="H13" s="50">
         <f>Summary!AB26</f>
-        <v>80.45097095349729</v>
+        <v>66.667936426690574</v>
       </c>
       <c r="I13" s="114">
         <v>37</v>
       </c>
+      <c r="J13" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="66">
-        <f>TubeLoading!F42</f>
-        <v>2445</v>
+        <f>TubeLoading!F44</f>
+        <v>1502</v>
       </c>
       <c r="B14" s="66" t="str">
-        <f>TubeLoading!A42</f>
-        <v>Tube N</v>
+        <f>TubeLoading!A44</f>
+        <v>Tube P</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D14" s="67">
         <v>45014</v>
@@ -10931,92 +10338,23 @@
         <v>140</v>
       </c>
       <c r="F14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G14" s="66">
-        <f>TubeLoading!J42</f>
+        <f>TubeLoading!J44</f>
         <v>4000</v>
       </c>
       <c r="H14" s="50">
         <f>Summary!AE26</f>
-        <v>73.835192341047971</v>
+        <v>71.313343562102091</v>
       </c>
       <c r="I14" s="115">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="66">
-        <f>TubeLoading!F43</f>
-        <v>2021</v>
-      </c>
-      <c r="B15" s="66" t="str">
-        <f>TubeLoading!A43</f>
-        <v>Tube O</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>202</v>
-      </c>
-      <c r="D15" s="67">
-        <v>45014</v>
-      </c>
-      <c r="E15">
-        <v>140</v>
-      </c>
-      <c r="F15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" s="66">
-        <f>TubeLoading!J43</f>
-        <v>3999.9999999999995</v>
-      </c>
-      <c r="H15" s="50">
-        <f>Summary!AH26</f>
-        <v>66.667936426690574</v>
-      </c>
-      <c r="I15" s="114">
-        <v>37</v>
-      </c>
-      <c r="J15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="66">
-        <f>TubeLoading!F44</f>
-        <v>1502</v>
-      </c>
-      <c r="B16" s="66" t="str">
-        <f>TubeLoading!A44</f>
-        <v>Tube P</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>202</v>
-      </c>
-      <c r="D16" s="67">
-        <v>45014</v>
-      </c>
-      <c r="E16">
-        <v>140</v>
-      </c>
-      <c r="F16" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="66">
-        <f>TubeLoading!J44</f>
-        <v>4000</v>
-      </c>
-      <c r="H16" s="50">
-        <f>Summary!AK26</f>
-        <v>71.313343562102091</v>
-      </c>
-      <c r="I16" s="115">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>207</v>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -12074,7 +11412,7 @@
         <v>1.6877187360000008</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -12099,7 +11437,7 @@
         <v>1.6811621760000008</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -12124,7 +11462,7 @@
         <v>1.6767911360000021</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -12149,7 +11487,7 @@
         <v>1.6693330490000005</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -12174,7 +11512,7 @@
         <v>1.6485706090000001</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -12199,7 +11537,7 @@
         <v>1.5556860090000004</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -12224,7 +11562,7 @@
         <v>1.3568036890000013</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -12249,7 +11587,7 @@
         <v>1.1338806490000017</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -14539,7 +13877,7 @@
         <v>1.6881558400000003</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -14564,7 +13902,7 @@
         <v>1.6826920400000009</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -14589,7 +13927,7 @@
         <v>1.6783210000000022</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -14614,7 +13952,7 @@
         <v>1.6706716799999999</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -14639,7 +13977,7 @@
         <v>1.6389816400000008</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -14664,7 +14002,7 @@
         <v>1.5165925199999997</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -14689,7 +14027,7 @@
         <v>1.2794635999999997</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -14714,7 +14052,7 @@
         <v>1.1013437200000009</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -17559,7 +16897,7 @@
         <v>119</v>
       </c>
       <c r="H14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -18222,7 +17560,7 @@
         <v>1.6923356470000002</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -18247,7 +17585,7 @@
         <v>1.6868718470000008</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -18272,7 +17610,7 @@
         <v>1.6803152870000009</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -18297,7 +17635,7 @@
         <v>1.6737587269999992</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -18322,7 +17660,7 @@
         <v>1.6529962870000006</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -18347,7 +17685,7 @@
         <v>1.5590189270000003</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -18372,7 +17710,7 @@
         <v>1.3481162470000019</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -18397,7 +17735,7 @@
         <v>1.1350280470000005</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -19625,10 +18963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA4E3B1-5772-4D1F-AF5A-033072A123CA}">
-  <dimension ref="A1:AK86"/>
+  <dimension ref="A1:AE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="12.45"/>
@@ -19643,9 +18981,9 @@
     <col min="12" max="16384" width="10.921875" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="12.9" thickTop="1">
+    <row r="1" spans="1:31" ht="12.9" thickTop="1">
       <c r="A1" s="62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B1" s="99">
         <f>TubeLoading!F29</f>
@@ -19696,105 +19034,81 @@
         <v>1515-conc</v>
       </c>
       <c r="N1" s="100">
-        <f>TubeLoading!F33</f>
-        <v>3193</v>
-      </c>
-      <c r="O1" s="101" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$33,"density")</f>
-        <v>3193-density</v>
-      </c>
-      <c r="P1" s="101" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$33,"conc")</f>
-        <v>3193-conc</v>
-      </c>
-      <c r="Q1" s="100">
-        <f>TubeLoading!F34</f>
-        <v>2383</v>
-      </c>
-      <c r="R1" s="101" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$34,"density")</f>
-        <v>2383-density</v>
-      </c>
-      <c r="S1" s="101" t="str">
-        <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$34,"conc")</f>
-        <v>2383-conc</v>
-      </c>
-      <c r="T1" s="100">
         <f>TubeLoading!F35</f>
         <v>3654</v>
       </c>
-      <c r="U1" s="101" t="str">
+      <c r="O1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$35,"density")</f>
         <v>3654-density</v>
       </c>
-      <c r="V1" s="101" t="str">
+      <c r="P1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$35,"conc")</f>
         <v>3654-conc</v>
       </c>
-      <c r="W1" s="100">
+      <c r="Q1" s="100">
         <f>TubeLoading!F36</f>
         <v>1794</v>
       </c>
-      <c r="X1" s="101" t="str">
+      <c r="R1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$36,"density")</f>
         <v>1794-density</v>
       </c>
-      <c r="Y1" s="101" t="str">
+      <c r="S1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$36,"conc")</f>
         <v>1794-conc</v>
       </c>
-      <c r="Z1" s="100">
+      <c r="T1" s="100">
         <f>TubeLoading!F41</f>
         <v>4016</v>
       </c>
-      <c r="AA1" s="101" t="str">
+      <c r="U1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$41,"density")</f>
         <v>4016-density</v>
       </c>
-      <c r="AB1" s="101" t="str">
+      <c r="V1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$41,"conc")</f>
         <v>4016-conc</v>
       </c>
-      <c r="AC1" s="100">
+      <c r="W1" s="100">
         <f>TubeLoading!F42</f>
         <v>2445</v>
       </c>
-      <c r="AD1" s="101" t="str">
+      <c r="X1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$42,"density")</f>
         <v>2445-density</v>
       </c>
-      <c r="AE1" s="101" t="str">
+      <c r="Y1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$42,"conc")</f>
         <v>2445-conc</v>
       </c>
-      <c r="AF1" s="100">
+      <c r="Z1" s="100">
         <f>TubeLoading!F43</f>
         <v>2021</v>
       </c>
-      <c r="AG1" s="101" t="str">
+      <c r="AA1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$43,"density")</f>
         <v>2021-density</v>
       </c>
-      <c r="AH1" s="101" t="str">
+      <c r="AB1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$43,"conc")</f>
         <v>2021-conc</v>
       </c>
-      <c r="AI1" s="100">
+      <c r="AC1" s="100">
         <f>TubeLoading!F44</f>
         <v>1502</v>
       </c>
-      <c r="AJ1" s="101" t="str">
+      <c r="AD1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$44,"density")</f>
         <v>1502-density</v>
       </c>
-      <c r="AK1" s="101" t="str">
+      <c r="AE1" s="101" t="str">
         <f>_xlfn.TEXTJOIN("-",TRUE,TubeLoading!$F$44,"conc")</f>
         <v>1502-conc</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:31">
       <c r="A2" s="62" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B2" s="119" t="s">
         <v>169</v>
@@ -19827,150 +19141,122 @@
       <c r="R2" s="117"/>
       <c r="S2" s="118"/>
       <c r="T2" s="116" t="s">
-        <v>176</v>
+        <v>5</v>
       </c>
       <c r="U2" s="117"/>
       <c r="V2" s="118"/>
       <c r="W2" s="116" t="s">
-        <v>177</v>
+        <v>23</v>
       </c>
       <c r="X2" s="117"/>
       <c r="Y2" s="118"/>
       <c r="Z2" s="116" t="s">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="AA2" s="117"/>
       <c r="AB2" s="118"/>
       <c r="AC2" s="116" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="AD2" s="117"/>
       <c r="AE2" s="118"/>
-      <c r="AF2" s="116" t="s">
-        <v>203</v>
-      </c>
-      <c r="AG2" s="117"/>
-      <c r="AH2" s="118"/>
-      <c r="AI2" s="116" t="s">
-        <v>204</v>
-      </c>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="118"/>
-    </row>
-    <row r="3" spans="1:37">
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" s="65" t="s">
         <v>173</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F3" s="64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G3" s="65" t="s">
         <v>173</v>
       </c>
       <c r="H3" s="63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I3" s="64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J3" s="65" t="s">
         <v>173</v>
       </c>
       <c r="K3" s="63" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M3" s="65" t="s">
         <v>173</v>
       </c>
       <c r="N3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P3" s="86" t="s">
         <v>173</v>
       </c>
       <c r="Q3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S3" s="86" t="s">
         <v>173</v>
       </c>
       <c r="T3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="V3" s="86" t="s">
         <v>173</v>
       </c>
       <c r="W3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="X3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Y3" s="86" t="s">
         <v>173</v>
       </c>
       <c r="Z3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AB3" s="86" t="s">
         <v>173</v>
       </c>
       <c r="AC3" s="84" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AD3" s="85" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AE3" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="AF3" s="84" t="s">
-        <v>188</v>
-      </c>
-      <c r="AG3" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="AH3" s="86" t="s">
-        <v>173</v>
-      </c>
-      <c r="AI3" s="84" t="s">
-        <v>188</v>
-      </c>
-      <c r="AJ3" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="AK3" s="86" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37">
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="56">
         <v>1</v>
       </c>
@@ -20019,95 +19305,73 @@
         <v>-2.5927305423049527E-2</v>
       </c>
       <c r="N4" s="69" t="str">
-        <f>'Tube E'!G2</f>
-        <v>A1</v>
-      </c>
-      <c r="O4" s="70">
-        <f>'Tube E'!F2</f>
-        <v>1.7626274340000005</v>
-      </c>
-      <c r="P4" s="71">
-        <v>-2.0463783997860068E-2</v>
-      </c>
-      <c r="Q4" s="69" t="str">
-        <f>'Tube F'!G2</f>
-        <v>G3</v>
-      </c>
-      <c r="R4" s="70">
-        <f>'Tube F'!F2</f>
-        <v>1.7557430459999992</v>
-      </c>
-      <c r="S4" s="71">
-        <v>-1.2482013580888102E-2</v>
-      </c>
-      <c r="T4" s="69" t="str">
         <f>'Tube G'!G2</f>
         <v>D6</v>
       </c>
-      <c r="U4" s="70">
+      <c r="O4" s="70">
         <f>'Tube G'!F2</f>
         <v>1.7556064510000002</v>
       </c>
-      <c r="V4" s="71">
+      <c r="P4" s="71">
         <v>6.3135528703066837E-2</v>
       </c>
-      <c r="W4" s="69" t="str">
+      <c r="Q4" s="69" t="str">
         <f>'Tube H'!G2</f>
         <v>C9</v>
       </c>
-      <c r="X4" s="70">
+      <c r="R4" s="70">
         <f>'Tube H'!F2</f>
         <v>1.7463453100000006</v>
       </c>
-      <c r="Y4" s="71">
+      <c r="S4" s="71">
         <v>4.1425655064496721E-3</v>
       </c>
-      <c r="Z4" s="69" t="str">
+      <c r="T4" s="69" t="str">
         <f>'Tube M'!G2</f>
         <v>A1</v>
       </c>
-      <c r="AA4" s="70">
+      <c r="U4" s="70">
         <f>'Tube M'!F2</f>
         <v>1.778417816000001</v>
       </c>
-      <c r="AB4" s="71">
+      <c r="V4" s="71">
         <v>-1.9260806273593511E-2</v>
       </c>
-      <c r="AC4" s="69" t="str">
+      <c r="W4" s="69" t="str">
         <f>'Tube N'!G2</f>
         <v>G3</v>
       </c>
-      <c r="AD4" s="70">
+      <c r="X4" s="70">
         <f>'Tube N'!F2</f>
         <v>1.7665886890000024</v>
       </c>
-      <c r="AE4" s="71">
+      <c r="Y4" s="71">
         <v>-3.631424088795001E-2</v>
       </c>
-      <c r="AF4" s="69" t="str">
+      <c r="Z4" s="69" t="str">
         <f>'Tube O'!G2</f>
         <v>D6</v>
       </c>
-      <c r="AG4" s="70">
+      <c r="AA4" s="70">
         <f>'Tube O'!F2</f>
         <v>1.7584203079999998</v>
       </c>
-      <c r="AH4" s="71">
+      <c r="AB4" s="71">
         <v>-2.2378046971212845E-2</v>
       </c>
-      <c r="AI4" s="69" t="str">
+      <c r="AC4" s="69" t="str">
         <f>'Tube P'!G2</f>
         <v>C9</v>
       </c>
-      <c r="AJ4" s="70">
+      <c r="AD4" s="70">
         <f>'Tube P'!F2</f>
         <v>1.756617254</v>
       </c>
-      <c r="AK4" s="71">
+      <c r="AE4" s="71">
         <v>-2.0268071547348245E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:31">
       <c r="A5" s="56">
         <v>2</v>
       </c>
@@ -20156,95 +19420,73 @@
         <v>-4.7293463991836454E-2</v>
       </c>
       <c r="N5" s="72" t="str">
-        <f>'Tube E'!G3</f>
-        <v>B1</v>
-      </c>
-      <c r="O5" s="73">
-        <f>'Tube E'!F3</f>
-        <v>1.7626274340000005</v>
-      </c>
-      <c r="P5" s="74">
-        <v>-5.3538839960976458E-4</v>
-      </c>
-      <c r="Q5" s="72" t="str">
-        <f>'Tube F'!G3</f>
-        <v>H3</v>
-      </c>
-      <c r="R5" s="73">
-        <f>'Tube F'!F3</f>
-        <v>1.7581197989999993</v>
-      </c>
-      <c r="S5" s="74">
-        <v>2.3851345744681399E-2</v>
-      </c>
-      <c r="T5" s="72" t="str">
         <f>'Tube G'!G3</f>
         <v>C6</v>
       </c>
-      <c r="U5" s="73">
+      <c r="O5" s="73">
         <f>'Tube G'!F3</f>
         <v>1.756699210999999</v>
       </c>
-      <c r="V5" s="74">
+      <c r="P5" s="74">
         <v>0.15211840212196873</v>
       </c>
-      <c r="W5" s="72" t="str">
+      <c r="Q5" s="72" t="str">
         <f>'Tube H'!G3</f>
         <v>D9</v>
       </c>
-      <c r="X5" s="73">
+      <c r="R5" s="73">
         <f>'Tube H'!F3</f>
         <v>1.7561801500000005</v>
       </c>
-      <c r="Y5" s="74">
+      <c r="S5" s="74">
         <v>3.1364586365325429E-2</v>
       </c>
-      <c r="Z5" s="72" t="str">
+      <c r="T5" s="72" t="str">
         <f>'Tube M'!G3</f>
         <v>B1</v>
       </c>
-      <c r="AA5" s="73">
+      <c r="U5" s="73">
         <f>'Tube M'!F3</f>
         <v>1.7696757360000017</v>
       </c>
-      <c r="AB5" s="74">
+      <c r="V5" s="74">
         <v>-9.0888505915609711E-3</v>
       </c>
-      <c r="AC5" s="72" t="str">
+      <c r="W5" s="72" t="str">
         <f>'Tube N'!G3</f>
         <v>H3</v>
       </c>
-      <c r="AD5" s="73">
+      <c r="X5" s="73">
         <f>'Tube N'!F3</f>
         <v>1.7654959290000019</v>
       </c>
-      <c r="AE5" s="74">
+      <c r="Y5" s="74">
         <v>-3.0937932732867681E-2</v>
       </c>
-      <c r="AF5" s="72" t="str">
+      <c r="Z5" s="72" t="str">
         <f>'Tube O'!G3</f>
         <v>C6</v>
       </c>
-      <c r="AG5" s="73">
+      <c r="AA5" s="73">
         <f>'Tube O'!F3</f>
         <v>1.7627913480000004</v>
       </c>
-      <c r="AH5" s="74">
+      <c r="AB5" s="74">
         <v>-2.2975089825000589E-2</v>
       </c>
-      <c r="AI5" s="72" t="str">
+      <c r="AC5" s="72" t="str">
         <f>'Tube P'!G3</f>
         <v>D9</v>
       </c>
-      <c r="AJ5" s="73">
+      <c r="AD5" s="73">
         <f>'Tube P'!F3</f>
         <v>1.763173814</v>
       </c>
-      <c r="AK5" s="74">
+      <c r="AE5" s="74">
         <v>-2.26125333696168E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:31">
       <c r="A6" s="56">
         <v>3</v>
       </c>
@@ -20293,95 +19535,73 @@
         <v>-4.6978705082012469E-2</v>
       </c>
       <c r="N6" s="72" t="str">
-        <f>'Tube E'!G4</f>
-        <v>C1</v>
-      </c>
-      <c r="O6" s="73">
-        <f>'Tube E'!F4</f>
-        <v>1.758256394</v>
-      </c>
-      <c r="P6" s="74">
-        <v>1.0608585303546176E-2</v>
-      </c>
-      <c r="Q6" s="72" t="str">
-        <f>'Tube F'!G4</f>
-        <v>H4</v>
-      </c>
-      <c r="R6" s="73">
-        <f>'Tube F'!F4</f>
-        <v>1.7548415189999993</v>
-      </c>
-      <c r="S6" s="74">
-        <v>9.6906363608471935E-2</v>
-      </c>
-      <c r="T6" s="72" t="str">
         <f>'Tube G'!G4</f>
         <v>B6</v>
       </c>
-      <c r="U6" s="73">
+      <c r="O6" s="73">
         <f>'Tube G'!F4</f>
         <v>1.7534209310000008</v>
       </c>
-      <c r="V6" s="74">
+      <c r="P6" s="74">
         <v>0.49708762670796364</v>
       </c>
-      <c r="W6" s="72" t="str">
+      <c r="Q6" s="72" t="str">
         <f>'Tube H'!G4</f>
         <v>E9</v>
       </c>
-      <c r="X6" s="73">
+      <c r="R6" s="73">
         <f>'Tube H'!F4</f>
         <v>1.7529018700000005</v>
       </c>
-      <c r="Y6" s="74">
+      <c r="S6" s="74">
         <v>8.4720704572724292E-2</v>
       </c>
-      <c r="Z6" s="72" t="str">
+      <c r="T6" s="72" t="str">
         <f>'Tube M'!G4</f>
         <v>C1</v>
       </c>
-      <c r="AA6" s="73">
+      <c r="U6" s="73">
         <f>'Tube M'!F4</f>
         <v>1.7653046960000012</v>
       </c>
-      <c r="AB6" s="74">
+      <c r="V6" s="74">
         <v>-1.07127253001656E-2</v>
       </c>
-      <c r="AC6" s="72" t="str">
+      <c r="W6" s="72" t="str">
         <f>'Tube N'!G4</f>
         <v>H4</v>
       </c>
-      <c r="AD6" s="73">
+      <c r="X6" s="73">
         <f>'Tube N'!F4</f>
         <v>1.762408881999999</v>
       </c>
-      <c r="AE6" s="74">
+      <c r="Y6" s="74">
         <v>-3.9780268731960007E-2</v>
       </c>
-      <c r="AF6" s="72" t="str">
+      <c r="Z6" s="72" t="str">
         <f>'Tube O'!G4</f>
         <v>B6</v>
       </c>
-      <c r="AG6" s="73">
+      <c r="AA6" s="73">
         <f>'Tube O'!F4</f>
         <v>1.7595130680000004</v>
       </c>
-      <c r="AH6" s="74">
+      <c r="AB6" s="74">
         <v>-1.28361843136513E-2</v>
       </c>
-      <c r="AI6" s="72" t="str">
+      <c r="AC6" s="72" t="str">
         <f>'Tube P'!G4</f>
         <v>E9</v>
       </c>
-      <c r="AJ6" s="73">
+      <c r="AD6" s="73">
         <f>'Tube P'!F4</f>
         <v>1.7609882940000006</v>
       </c>
-      <c r="AK6" s="74">
+      <c r="AE6" s="74">
         <v>-2.4975540027317691E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:31">
       <c r="A7" s="56">
         <v>4</v>
       </c>
@@ -20430,95 +19650,73 @@
         <v>-3.9753029952670667E-2</v>
       </c>
       <c r="N7" s="72" t="str">
-        <f>'Tube E'!G5</f>
-        <v>D1</v>
-      </c>
-      <c r="O7" s="73">
-        <f>'Tube E'!F5</f>
-        <v>1.7527925940000006</v>
-      </c>
-      <c r="P7" s="74">
-        <v>0.10043130380465427</v>
-      </c>
-      <c r="Q7" s="72" t="str">
-        <f>'Tube F'!G5</f>
-        <v>G4</v>
-      </c>
-      <c r="R7" s="73">
-        <f>'Tube F'!F5</f>
-        <v>1.7493777189999999</v>
-      </c>
-      <c r="S7" s="74">
-        <v>0.22550491251158367</v>
-      </c>
-      <c r="T7" s="72" t="str">
         <f>'Tube G'!G5</f>
         <v>A6</v>
       </c>
-      <c r="U7" s="73">
+      <c r="O7" s="73">
         <f>'Tube G'!F5</f>
         <v>1.7494323570000017</v>
       </c>
-      <c r="V7" s="74">
+      <c r="P7" s="74">
         <v>0.82814741683358373</v>
       </c>
-      <c r="W7" s="72" t="str">
+      <c r="Q7" s="72" t="str">
         <f>'Tube H'!G5</f>
         <v>F9</v>
       </c>
-      <c r="X7" s="73">
+      <c r="R7" s="73">
         <f>'Tube H'!F5</f>
         <v>1.7498148230000012</v>
       </c>
-      <c r="Y7" s="74">
+      <c r="S7" s="74">
         <v>0.20980255047667609</v>
       </c>
-      <c r="Z7" s="72" t="str">
+      <c r="T7" s="72" t="str">
         <f>'Tube M'!G5</f>
         <v>D1</v>
       </c>
-      <c r="AA7" s="73">
+      <c r="U7" s="73">
         <f>'Tube M'!F5</f>
         <v>1.7609336559999988</v>
       </c>
-      <c r="AB7" s="74">
+      <c r="V7" s="74">
         <v>2.5181330286629337E-2</v>
       </c>
-      <c r="AC7" s="72" t="str">
+      <c r="W7" s="72" t="str">
         <f>'Tube N'!G5</f>
         <v>G4</v>
       </c>
-      <c r="AD7" s="73">
+      <c r="X7" s="73">
         <f>'Tube N'!F5</f>
         <v>1.7591306020000008</v>
       </c>
-      <c r="AE7" s="74">
+      <c r="Y7" s="74">
         <v>-1.3137761498474376E-2</v>
       </c>
-      <c r="AF7" s="72" t="str">
+      <c r="Z7" s="72" t="str">
         <f>'Tube O'!G5</f>
         <v>A6</v>
       </c>
-      <c r="AG7" s="73">
+      <c r="AA7" s="73">
         <f>'Tube O'!F5</f>
         <v>1.754049268000001</v>
       </c>
-      <c r="AH7" s="74">
+      <c r="AB7" s="74">
         <v>-4.2167280137465207E-3</v>
       </c>
-      <c r="AI7" s="72" t="str">
+      <c r="AC7" s="72" t="str">
         <f>'Tube P'!G5</f>
         <v>F9</v>
       </c>
-      <c r="AJ7" s="73">
+      <c r="AD7" s="73">
         <f>'Tube P'!F5</f>
         <v>1.7555244940000012</v>
       </c>
-      <c r="AK7" s="74">
+      <c r="AE7" s="74">
         <v>-4.289607887565162E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:31">
       <c r="A8" s="56">
         <v>5</v>
       </c>
@@ -20567,95 +19765,73 @@
         <v>-1.256568155723841E-2</v>
       </c>
       <c r="N8" s="72" t="str">
-        <f>'Tube E'!G6</f>
-        <v>E1</v>
-      </c>
-      <c r="O8" s="73">
-        <f>'Tube E'!F6</f>
-        <v>1.7464272670000014</v>
-      </c>
-      <c r="P8" s="74">
-        <v>0.175360529597648</v>
-      </c>
-      <c r="Q8" s="72" t="str">
-        <f>'Tube F'!G6</f>
-        <v>F4</v>
-      </c>
-      <c r="R8" s="73">
-        <f>'Tube F'!F6</f>
-        <v>1.7439139190000006</v>
-      </c>
-      <c r="S8" s="74">
-        <v>0.70629344241902603</v>
-      </c>
-      <c r="T8" s="72" t="str">
         <f>'Tube G'!G6</f>
         <v>A7</v>
       </c>
-      <c r="U8" s="73">
+      <c r="O8" s="73">
         <f>'Tube G'!F6</f>
         <v>1.7446788510000015</v>
       </c>
-      <c r="V8" s="74">
+      <c r="P8" s="74">
         <v>1.3717738549680407</v>
       </c>
-      <c r="W8" s="72" t="str">
+      <c r="Q8" s="72" t="str">
         <f>'Tube H'!G6</f>
         <v>G9</v>
       </c>
-      <c r="X8" s="73">
+      <c r="R8" s="73">
         <f>'Tube H'!F6</f>
         <v>1.7443510230000019</v>
       </c>
-      <c r="Y8" s="74">
+      <c r="S8" s="74">
         <v>0.53246092780398058</v>
       </c>
-      <c r="Z8" s="72" t="str">
+      <c r="T8" s="72" t="str">
         <f>'Tube M'!G6</f>
         <v>E1</v>
       </c>
-      <c r="AA8" s="73">
+      <c r="U8" s="73">
         <f>'Tube M'!F6</f>
         <v>1.7543770960000007</v>
       </c>
-      <c r="AB8" s="74">
+      <c r="V8" s="74">
         <v>0.20306859261396207</v>
       </c>
-      <c r="AC8" s="72" t="str">
+      <c r="W8" s="72" t="str">
         <f>'Tube N'!G6</f>
         <v>F4</v>
       </c>
-      <c r="AD8" s="73">
+      <c r="X8" s="73">
         <f>'Tube N'!F6</f>
         <v>1.7514812820000003</v>
       </c>
-      <c r="AE8" s="74">
+      <c r="Y8" s="74">
         <v>-3.3201279753309033E-2</v>
       </c>
-      <c r="AF8" s="72" t="str">
+      <c r="Z8" s="72" t="str">
         <f>'Tube O'!G6</f>
         <v>A7</v>
       </c>
-      <c r="AG8" s="73">
+      <c r="AA8" s="73">
         <f>'Tube O'!F6</f>
         <v>1.7507709880000011</v>
       </c>
-      <c r="AH8" s="74">
+      <c r="AB8" s="74">
         <v>1.1170875569129692E-2</v>
       </c>
-      <c r="AI8" s="72" t="str">
+      <c r="AC8" s="72" t="str">
         <f>'Tube P'!G6</f>
         <v>G9</v>
       </c>
-      <c r="AJ8" s="73">
+      <c r="AD8" s="73">
         <f>'Tube P'!F6</f>
         <v>1.7511534540000007</v>
       </c>
-      <c r="AK8" s="74">
+      <c r="AE8" s="74">
         <v>4.8797633538395085E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:31">
       <c r="A9" s="56">
         <v>6</v>
       </c>
@@ -20704,95 +19880,73 @@
         <v>-2.2468599358782759E-2</v>
       </c>
       <c r="N9" s="72" t="str">
-        <f>'Tube E'!G7</f>
-        <v>F1</v>
-      </c>
-      <c r="O9" s="73">
-        <f>'Tube E'!F7</f>
-        <v>1.7398707070000015</v>
-      </c>
-      <c r="P9" s="74">
-        <v>0.51863065556540644</v>
-      </c>
-      <c r="Q9" s="72" t="str">
-        <f>'Tube F'!G7</f>
-        <v>E4</v>
-      </c>
-      <c r="R9" s="73">
-        <f>'Tube F'!F7</f>
-        <v>1.7373573589999989</v>
-      </c>
-      <c r="S9" s="74">
-        <v>1.6691083790296721</v>
-      </c>
-      <c r="T9" s="72" t="str">
         <f>'Tube G'!G7</f>
         <v>B7</v>
       </c>
-      <c r="U9" s="73">
+      <c r="O9" s="73">
         <f>'Tube G'!F7</f>
         <v>1.7383135239999987</v>
       </c>
-      <c r="V9" s="74">
+      <c r="P9" s="74">
         <v>2.7118808343174479</v>
       </c>
-      <c r="W9" s="72" t="str">
+      <c r="Q9" s="72" t="str">
         <f>'Tube H'!G7</f>
         <v>H9</v>
       </c>
-      <c r="X9" s="73">
+      <c r="R9" s="73">
         <f>'Tube H'!F7</f>
         <v>1.7377944630000002</v>
       </c>
-      <c r="Y9" s="75">
+      <c r="S9" s="75">
         <v>1.2094760523075958</v>
       </c>
-      <c r="Z9" s="72" t="str">
+      <c r="T9" s="72" t="str">
         <f>'Tube M'!G7</f>
         <v>F1</v>
       </c>
-      <c r="AA9" s="73">
+      <c r="U9" s="73">
         <f>'Tube M'!F7</f>
         <v>1.746727776000002</v>
       </c>
-      <c r="AB9" s="74">
+      <c r="V9" s="74">
         <v>0.48310675943885589</v>
       </c>
-      <c r="AC9" s="72" t="str">
+      <c r="W9" s="72" t="str">
         <f>'Tube N'!G7</f>
         <v>E4</v>
       </c>
-      <c r="AD9" s="73">
+      <c r="X9" s="73">
         <f>'Tube N'!F7</f>
         <v>1.7449247220000021</v>
       </c>
-      <c r="AE9" s="74">
+      <c r="Y9" s="74">
         <v>-3.6907362884874887E-3</v>
       </c>
-      <c r="AF9" s="72" t="str">
+      <c r="Z9" s="72" t="str">
         <f>'Tube O'!G7</f>
         <v>B7</v>
       </c>
-      <c r="AG9" s="73">
+      <c r="AA9" s="73">
         <f>'Tube O'!F7</f>
         <v>1.7442144280000011</v>
       </c>
-      <c r="AH9" s="74">
+      <c r="AB9" s="74">
         <v>9.1829408963584047E-2</v>
       </c>
-      <c r="AI9" s="72" t="str">
+      <c r="AC9" s="72" t="str">
         <f>'Tube P'!G7</f>
         <v>H9</v>
       </c>
-      <c r="AJ9" s="73">
+      <c r="AD9" s="73">
         <f>'Tube P'!F7</f>
         <v>1.7445968940000025</v>
       </c>
-      <c r="AK9" s="74">
+      <c r="AE9" s="74">
         <v>0.13751671711228819</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:31">
       <c r="A10" s="56">
         <v>7</v>
       </c>
@@ -20841,95 +19995,73 @@
         <v>5.6249391568224415E-2</v>
       </c>
       <c r="N10" s="72" t="str">
-        <f>'Tube E'!G8</f>
-        <v>G1</v>
-      </c>
-      <c r="O10" s="73">
-        <f>'Tube E'!F8</f>
-        <v>1.7354996669999991</v>
-      </c>
-      <c r="P10" s="74">
-        <v>1.2204466196133288</v>
-      </c>
-      <c r="Q10" s="72" t="str">
-        <f>'Tube F'!G8</f>
-        <v>D4</v>
-      </c>
-      <c r="R10" s="73">
-        <f>'Tube F'!F8</f>
-        <v>1.7318935589999995</v>
-      </c>
-      <c r="S10" s="74">
-        <v>3.6870802157983049</v>
-      </c>
-      <c r="T10" s="72" t="str">
         <f>'Tube G'!G8</f>
         <v>C7</v>
       </c>
-      <c r="U10" s="73">
+      <c r="O10" s="73">
         <f>'Tube G'!F8</f>
         <v>1.7328497239999994</v>
       </c>
-      <c r="V10" s="74">
+      <c r="P10" s="74">
         <v>4.476840392034898</v>
       </c>
-      <c r="W10" s="72" t="str">
+      <c r="Q10" s="72" t="str">
         <f>'Tube H'!G8</f>
         <v>H10</v>
       </c>
-      <c r="X10" s="73">
+      <c r="R10" s="73">
         <f>'Tube H'!F8</f>
         <v>1.7323306630000008</v>
       </c>
-      <c r="Y10" s="75">
+      <c r="S10" s="75">
         <v>2.670654578974172</v>
       </c>
-      <c r="Z10" s="72" t="str">
+      <c r="T10" s="72" t="str">
         <f>'Tube M'!G8</f>
         <v>G1</v>
       </c>
-      <c r="AA10" s="73">
+      <c r="U10" s="73">
         <f>'Tube M'!F8</f>
         <v>1.7401712160000002</v>
       </c>
-      <c r="AB10" s="74">
+      <c r="V10" s="74">
         <v>1.0814671128458431</v>
       </c>
-      <c r="AC10" s="72" t="str">
+      <c r="W10" s="72" t="str">
         <f>'Tube N'!G8</f>
         <v>D4</v>
       </c>
-      <c r="AD10" s="73">
+      <c r="X10" s="73">
         <f>'Tube N'!F8</f>
         <v>1.7383681620000004</v>
       </c>
-      <c r="AE10" s="74">
+      <c r="Y10" s="74">
         <v>0.10572731620310376</v>
       </c>
-      <c r="AF10" s="72" t="str">
+      <c r="Z10" s="72" t="str">
         <f>'Tube O'!G8</f>
         <v>C7</v>
       </c>
-      <c r="AG10" s="73">
+      <c r="AA10" s="73">
         <f>'Tube O'!F8</f>
         <v>1.7376578679999994</v>
       </c>
-      <c r="AH10" s="74">
+      <c r="AB10" s="74">
         <v>0.3487931242006681</v>
       </c>
-      <c r="AI10" s="72" t="str">
+      <c r="AC10" s="72" t="str">
         <f>'Tube P'!G8</f>
         <v>H10</v>
       </c>
-      <c r="AJ10" s="73">
+      <c r="AD10" s="73">
         <f>'Tube P'!F8</f>
         <v>1.7391330939999996</v>
       </c>
-      <c r="AK10" s="75">
+      <c r="AE10" s="75">
         <v>0.36713105098143145</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:31">
       <c r="A11" s="56">
         <v>8</v>
       </c>
@@ -20978,95 +20110,73 @@
         <v>1.3949642302538967</v>
       </c>
       <c r="N11" s="72" t="str">
-        <f>'Tube E'!G9</f>
-        <v>H1</v>
-      </c>
-      <c r="O11" s="73">
-        <f>'Tube E'!F9</f>
-        <v>1.7291343399999999</v>
-      </c>
-      <c r="P11" s="74">
-        <v>2.9027148760908119</v>
-      </c>
-      <c r="Q11" s="72" t="str">
-        <f>'Tube F'!G9</f>
-        <v>C4</v>
-      </c>
-      <c r="R11" s="73">
-        <f>'Tube F'!F9</f>
-        <v>1.7255282320000003</v>
-      </c>
-      <c r="S11" s="74">
-        <v>7.2523410638667016</v>
-      </c>
-      <c r="T11" s="72" t="str">
         <f>'Tube G'!G9</f>
         <v>D7</v>
       </c>
-      <c r="U11" s="73">
+      <c r="O11" s="73">
         <f>'Tube G'!F9</f>
         <v>1.7262931640000012</v>
       </c>
-      <c r="V11" s="74">
+      <c r="P11" s="74">
         <v>6.9607528696289513</v>
       </c>
-      <c r="W11" s="72" t="str">
+      <c r="Q11" s="72" t="str">
         <f>'Tube H'!G9</f>
         <v>G10</v>
       </c>
-      <c r="X11" s="73">
+      <c r="R11" s="73">
         <f>'Tube H'!F9</f>
         <v>1.7268668630000015</v>
       </c>
-      <c r="Y11" s="75">
+      <c r="S11" s="75">
         <v>7.8226424013937317</v>
       </c>
-      <c r="Z11" s="72" t="str">
+      <c r="T11" s="72" t="str">
         <f>'Tube M'!G9</f>
         <v>H1</v>
       </c>
-      <c r="AA11" s="73">
+      <c r="U11" s="73">
         <f>'Tube M'!F9</f>
         <v>1.7336146560000003</v>
       </c>
-      <c r="AB11" s="74">
+      <c r="V11" s="74">
         <v>3.4931326444996196</v>
       </c>
-      <c r="AC11" s="72" t="str">
+      <c r="W11" s="72" t="str">
         <f>'Tube N'!G9</f>
         <v>C4</v>
       </c>
-      <c r="AD11" s="73">
+      <c r="X11" s="73">
         <f>'Tube N'!F9</f>
         <v>1.7329043620000011</v>
       </c>
-      <c r="AE11" s="74">
+      <c r="Y11" s="74">
         <v>1.3466151722515773</v>
       </c>
-      <c r="AF11" s="72" t="str">
+      <c r="Z11" s="72" t="str">
         <f>'Tube O'!G9</f>
         <v>D7</v>
       </c>
-      <c r="AG11" s="73">
+      <c r="AA11" s="73">
         <f>'Tube O'!F9</f>
         <v>1.7301997810000014</v>
       </c>
-      <c r="AH11" s="74">
+      <c r="AB11" s="74">
         <v>2.1376134445432378</v>
       </c>
-      <c r="AI11" s="72" t="str">
+      <c r="AC11" s="72" t="str">
         <f>'Tube P'!G9</f>
         <v>G10</v>
       </c>
-      <c r="AJ11" s="73">
+      <c r="AD11" s="73">
         <f>'Tube P'!F9</f>
         <v>1.7325765340000014</v>
       </c>
-      <c r="AK11" s="75">
+      <c r="AE11" s="75">
         <v>1.3773724794825835</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:31">
       <c r="A12" s="56">
         <v>9</v>
       </c>
@@ -21115,95 +20225,73 @@
         <v>14.277514778188879</v>
       </c>
       <c r="N12" s="72" t="str">
-        <f>'Tube E'!G10</f>
-        <v>H2</v>
-      </c>
-      <c r="O12" s="73">
-        <f>'Tube E'!F10</f>
-        <v>1.7225777799999999</v>
-      </c>
-      <c r="P12" s="74">
-        <v>7.0237378781819473</v>
-      </c>
-      <c r="Q12" s="72" t="str">
-        <f>'Tube F'!G10</f>
-        <v>B4</v>
-      </c>
-      <c r="R12" s="73">
-        <f>'Tube F'!F10</f>
-        <v>1.7200644320000009</v>
-      </c>
-      <c r="S12" s="74">
-        <v>16.462006311442085</v>
-      </c>
-      <c r="T12" s="72" t="str">
         <f>'Tube G'!G10</f>
         <v>E7</v>
       </c>
-      <c r="U12" s="73">
+      <c r="O12" s="73">
         <f>'Tube G'!F10</f>
         <v>1.7208293640000019</v>
       </c>
-      <c r="V12" s="74">
+      <c r="P12" s="74">
         <v>13.600594508199576</v>
       </c>
-      <c r="W12" s="72" t="str">
+      <c r="Q12" s="72" t="str">
         <f>'Tube H'!G10</f>
         <v>F10</v>
       </c>
-      <c r="X12" s="73">
+      <c r="R12" s="73">
         <f>'Tube H'!F10</f>
         <v>1.7203103030000015</v>
       </c>
-      <c r="Y12" s="75">
+      <c r="S12" s="75">
         <v>16.825580113159116</v>
       </c>
-      <c r="Z12" s="72" t="str">
+      <c r="T12" s="72" t="str">
         <f>'Tube M'!G10</f>
         <v>H2</v>
       </c>
-      <c r="AA12" s="73">
+      <c r="U12" s="73">
         <f>'Tube M'!F10</f>
         <v>1.7292436160000015</v>
       </c>
-      <c r="AB12" s="74">
+      <c r="V12" s="74">
         <v>9.9684851382542998</v>
       </c>
-      <c r="AC12" s="72" t="str">
+      <c r="W12" s="72" t="str">
         <f>'Tube N'!G10</f>
         <v>B4</v>
       </c>
-      <c r="AD12" s="73">
+      <c r="X12" s="73">
         <f>'Tube N'!F10</f>
         <v>1.7274405620000017</v>
       </c>
-      <c r="AE12" s="74">
+      <c r="Y12" s="74">
         <v>11.944523832149699</v>
       </c>
-      <c r="AF12" s="72" t="str">
+      <c r="Z12" s="72" t="str">
         <f>'Tube O'!G10</f>
         <v>E7</v>
       </c>
-      <c r="AG12" s="73">
+      <c r="AA12" s="73">
         <f>'Tube O'!F10</f>
         <v>1.724735981000002</v>
       </c>
-      <c r="AH12" s="74">
+      <c r="AB12" s="74">
         <v>13.812288942181334</v>
       </c>
-      <c r="AI12" s="72" t="str">
+      <c r="AC12" s="72" t="str">
         <f>'Tube P'!G10</f>
         <v>F10</v>
       </c>
-      <c r="AJ12" s="73">
+      <c r="AD12" s="73">
         <f>'Tube P'!F10</f>
         <v>1.7271127340000021</v>
       </c>
-      <c r="AK12" s="75">
+      <c r="AE12" s="75">
         <v>8.3925853727849447</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:31">
       <c r="A13" s="56">
         <v>10</v>
       </c>
@@ -21252,95 +20340,73 @@
         <v>18.110864252641065</v>
       </c>
       <c r="N13" s="72" t="str">
-        <f>'Tube E'!G11</f>
-        <v>G2</v>
-      </c>
-      <c r="O13" s="73">
-        <f>'Tube E'!F11</f>
-        <v>1.7171139799999988</v>
-      </c>
-      <c r="P13" s="75">
-        <v>11.613331556357783</v>
-      </c>
-      <c r="Q13" s="72" t="str">
-        <f>'Tube F'!G11</f>
-        <v>A4</v>
-      </c>
-      <c r="R13" s="73">
-        <f>'Tube F'!F11</f>
-        <v>1.7146006319999998</v>
-      </c>
-      <c r="S13" s="74">
-        <v>18.7283074693526</v>
-      </c>
-      <c r="T13" s="72" t="str">
         <f>'Tube G'!G11</f>
         <v>F7</v>
       </c>
-      <c r="U13" s="73">
+      <c r="O13" s="73">
         <f>'Tube G'!F11</f>
         <v>1.7131800439999996</v>
       </c>
-      <c r="V13" s="74">
+      <c r="P13" s="74">
         <v>11.76713976644281</v>
       </c>
-      <c r="W13" s="72" t="str">
+      <c r="Q13" s="72" t="str">
         <f>'Tube H'!G11</f>
         <v>E10</v>
       </c>
-      <c r="X13" s="73">
+      <c r="R13" s="73">
         <f>'Tube H'!F11</f>
         <v>1.7150377359999993</v>
       </c>
-      <c r="Y13" s="75">
+      <c r="S13" s="75">
         <v>17.212606027150656</v>
       </c>
-      <c r="Z13" s="72" t="str">
+      <c r="T13" s="72" t="str">
         <f>'Tube M'!G11</f>
         <v>G2</v>
       </c>
-      <c r="AA13" s="73">
+      <c r="U13" s="73">
         <f>'Tube M'!F11</f>
         <v>1.7226870560000016</v>
       </c>
-      <c r="AB13" s="74">
+      <c r="V13" s="74">
         <v>21.450682597248576</v>
       </c>
-      <c r="AC13" s="72" t="str">
+      <c r="W13" s="72" t="str">
         <f>'Tube N'!G11</f>
         <v>A4</v>
       </c>
-      <c r="AD13" s="73">
+      <c r="X13" s="73">
         <f>'Tube N'!F11</f>
         <v>1.7210752350000025</v>
       </c>
-      <c r="AE13" s="74">
+      <c r="Y13" s="74">
         <v>22.29222163583761</v>
       </c>
-      <c r="AF13" s="72" t="str">
+      <c r="Z13" s="72" t="str">
         <f>'Tube O'!G11</f>
         <v>F7</v>
       </c>
-      <c r="AG13" s="73">
+      <c r="AA13" s="73">
         <f>'Tube O'!F11</f>
         <v>1.7181794210000003</v>
       </c>
-      <c r="AH13" s="74">
+      <c r="AB13" s="74">
         <v>18.234916730350577</v>
       </c>
-      <c r="AI13" s="72" t="str">
+      <c r="AC13" s="72" t="str">
         <f>'Tube P'!G11</f>
         <v>E10</v>
       </c>
-      <c r="AJ13" s="73">
+      <c r="AD13" s="73">
         <f>'Tube P'!F11</f>
         <v>1.7205561740000004</v>
       </c>
-      <c r="AK13" s="74">
+      <c r="AE13" s="74">
         <v>16.185376531622445</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:31">
       <c r="A14" s="56">
         <v>11</v>
       </c>
@@ -21389,95 +20455,73 @@
         <v>12.059390896181178</v>
       </c>
       <c r="N14" s="72" t="str">
-        <f>'Tube E'!G12</f>
-        <v>F2</v>
-      </c>
-      <c r="O14" s="73">
-        <f>'Tube E'!F12</f>
-        <v>1.7105574199999989</v>
-      </c>
-      <c r="P14" s="75">
-        <v>9.4605341772915512</v>
-      </c>
-      <c r="Q14" s="72" t="str">
-        <f>'Tube F'!G12</f>
-        <v>A5</v>
-      </c>
-      <c r="R14" s="73">
-        <f>'Tube F'!F12</f>
-        <v>1.7102295919999992</v>
-      </c>
-      <c r="S14" s="74">
-        <v>11.907065732067259</v>
-      </c>
-      <c r="T14" s="72" t="str">
         <f>'Tube G'!G12</f>
         <v>G7</v>
       </c>
-      <c r="U14" s="73">
+      <c r="O14" s="73">
         <f>'Tube G'!F12</f>
         <v>1.7088090040000008</v>
       </c>
-      <c r="V14" s="74">
+      <c r="P14" s="74">
         <v>9.3274810221449211</v>
       </c>
-      <c r="W14" s="72" t="str">
+      <c r="Q14" s="72" t="str">
         <f>'Tube H'!G12</f>
         <v>D10</v>
       </c>
-      <c r="X14" s="73">
+      <c r="R14" s="73">
         <f>'Tube H'!F12</f>
         <v>1.709573936</v>
       </c>
-      <c r="Y14" s="75">
+      <c r="S14" s="75">
         <v>12.502931635667879</v>
       </c>
-      <c r="Z14" s="72" t="str">
+      <c r="T14" s="72" t="str">
         <f>'Tube M'!G12</f>
         <v>F2</v>
       </c>
-      <c r="AA14" s="73">
+      <c r="U14" s="73">
         <f>'Tube M'!F12</f>
         <v>1.7161304959999999</v>
       </c>
-      <c r="AB14" s="74">
+      <c r="V14" s="74">
         <v>18.324604676134882</v>
       </c>
-      <c r="AC14" s="72" t="str">
+      <c r="W14" s="72" t="str">
         <f>'Tube N'!G12</f>
         <v>A5</v>
       </c>
-      <c r="AD14" s="73">
+      <c r="X14" s="73">
         <f>'Tube N'!F12</f>
         <v>1.7167041950000002</v>
       </c>
-      <c r="AE14" s="74">
+      <c r="Y14" s="74">
         <v>18.235797641953198</v>
       </c>
-      <c r="AF14" s="72" t="str">
+      <c r="Z14" s="72" t="str">
         <f>'Tube O'!G12</f>
         <v>G7</v>
       </c>
-      <c r="AG14" s="73">
+      <c r="AA14" s="73">
         <f>'Tube O'!F12</f>
         <v>1.712715621000001</v>
       </c>
-      <c r="AH14" s="74">
+      <c r="AB14" s="74">
         <v>15.82570681100089</v>
       </c>
-      <c r="AI14" s="72" t="str">
+      <c r="AC14" s="72" t="str">
         <f>'Tube P'!G12</f>
         <v>D10</v>
       </c>
-      <c r="AJ14" s="73">
+      <c r="AD14" s="73">
         <f>'Tube P'!F12</f>
         <v>1.715092374000001</v>
       </c>
-      <c r="AK14" s="76">
+      <c r="AE14" s="76">
         <v>19.022443992235285</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:31">
       <c r="A15" s="56">
         <v>12</v>
       </c>
@@ -21526,95 +20570,73 @@
         <v>6.1758795646432132</v>
       </c>
       <c r="N15" s="72" t="str">
-        <f>'Tube E'!G13</f>
-        <v>E2</v>
-      </c>
-      <c r="O15" s="73">
-        <f>'Tube E'!F13</f>
-        <v>1.7050936199999995</v>
-      </c>
-      <c r="P15" s="75">
-        <v>5.3960084085803111</v>
-      </c>
-      <c r="Q15" s="72" t="str">
-        <f>'Tube F'!G13</f>
-        <v>B5</v>
-      </c>
-      <c r="R15" s="73">
-        <f>'Tube F'!F13</f>
-        <v>1.7047657919999999</v>
-      </c>
-      <c r="S15" s="74">
-        <v>6.8807231378408487</v>
-      </c>
-      <c r="T15" s="72" t="str">
         <f>'Tube G'!G13</f>
         <v>H7</v>
       </c>
-      <c r="U15" s="73">
+      <c r="O15" s="73">
         <f>'Tube G'!F13</f>
         <v>1.7035364370000003</v>
       </c>
-      <c r="V15" s="74">
+      <c r="P15" s="74">
         <v>6.458357908874663</v>
       </c>
-      <c r="W15" s="72" t="str">
+      <c r="Q15" s="72" t="str">
         <f>'Tube H'!G13</f>
         <v>C10</v>
       </c>
-      <c r="X15" s="73">
+      <c r="R15" s="73">
         <f>'Tube H'!F13</f>
         <v>1.7030173760000018</v>
       </c>
-      <c r="Y15" s="74">
+      <c r="S15" s="74">
         <v>6.4920750888033103</v>
       </c>
-      <c r="Z15" s="72" t="str">
+      <c r="T15" s="72" t="str">
         <f>'Tube M'!G13</f>
         <v>E2</v>
       </c>
-      <c r="AA15" s="73">
+      <c r="U15" s="73">
         <f>'Tube M'!F13</f>
         <v>1.7117594560000011</v>
       </c>
-      <c r="AB15" s="74">
+      <c r="V15" s="74">
         <v>13.158090764632249</v>
       </c>
-      <c r="AC15" s="72" t="str">
+      <c r="W15" s="72" t="str">
         <f>'Tube N'!G13</f>
         <v>B5</v>
       </c>
-      <c r="AD15" s="73">
+      <c r="X15" s="73">
         <f>'Tube N'!F13</f>
         <v>1.7101476350000002</v>
       </c>
-      <c r="AE15" s="74">
+      <c r="Y15" s="74">
         <v>11.569216695762584</v>
       </c>
-      <c r="AF15" s="72" t="str">
+      <c r="Z15" s="72" t="str">
         <f>'Tube O'!G13</f>
         <v>H7</v>
       </c>
-      <c r="AG15" s="73">
+      <c r="AA15" s="73">
         <f>'Tube O'!F13</f>
         <v>1.7072518210000016</v>
       </c>
-      <c r="AH15" s="74">
+      <c r="AB15" s="74">
         <v>9.5022800744590743</v>
       </c>
-      <c r="AI15" s="72" t="str">
+      <c r="AC15" s="72" t="str">
         <f>'Tube P'!G13</f>
         <v>C10</v>
       </c>
-      <c r="AJ15" s="73">
+      <c r="AD15" s="73">
         <f>'Tube P'!F13</f>
         <v>1.7096285740000017</v>
       </c>
-      <c r="AK15" s="76">
+      <c r="AE15" s="76">
         <v>13.873540936065636</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:31">
       <c r="A16" s="56">
         <v>13</v>
       </c>
@@ -21663,95 +20685,73 @@
         <v>2.062644497157772</v>
       </c>
       <c r="N16" s="72" t="str">
-        <f>'Tube E'!G14</f>
-        <v>D2</v>
-      </c>
-      <c r="O16" s="73">
-        <f>'Tube E'!F14</f>
-        <v>1.6996298200000002</v>
-      </c>
-      <c r="P16" s="75">
-        <v>2.581010398673115</v>
-      </c>
-      <c r="Q16" s="72" t="str">
-        <f>'Tube F'!G14</f>
-        <v>C5</v>
-      </c>
-      <c r="R16" s="73">
-        <f>'Tube F'!F14</f>
-        <v>1.6982092320000017</v>
-      </c>
-      <c r="S16" s="74">
-        <v>3.1848577497107544</v>
-      </c>
-      <c r="T16" s="72" t="str">
         <f>'Tube G'!G14</f>
         <v>H8</v>
       </c>
-      <c r="U16" s="73">
+      <c r="O16" s="73">
         <f>'Tube G'!F14</f>
         <v>1.698072637000001</v>
       </c>
-      <c r="V16" s="74">
+      <c r="P16" s="74">
         <v>2.0084376577031704</v>
       </c>
-      <c r="W16" s="72" t="str">
+      <c r="Q16" s="72" t="str">
         <f>'Tube H'!G14</f>
         <v>B10</v>
       </c>
-      <c r="X16" s="73">
+      <c r="R16" s="73">
         <f>'Tube H'!F14</f>
         <v>1.6964608160000001</v>
       </c>
-      <c r="Y16" s="74">
+      <c r="S16" s="74">
         <v>2.6712828920512535</v>
       </c>
-      <c r="Z16" s="72" t="str">
+      <c r="T16" s="72" t="str">
         <f>'Tube M'!G14</f>
         <v>D2</v>
       </c>
-      <c r="AA16" s="73">
+      <c r="U16" s="73">
         <f>'Tube M'!F14</f>
         <v>1.7052028960000012</v>
       </c>
-      <c r="AB16" s="74">
+      <c r="V16" s="74">
         <v>6.295960012504989</v>
       </c>
-      <c r="AC16" s="72" t="str">
+      <c r="W16" s="72" t="str">
         <f>'Tube N'!G14</f>
         <v>C5</v>
       </c>
-      <c r="AD16" s="73">
+      <c r="X16" s="73">
         <f>'Tube N'!F14</f>
         <v>1.7046838350000009</v>
       </c>
-      <c r="AE16" s="74">
+      <c r="Y16" s="74">
         <v>4.1424341088283043</v>
       </c>
-      <c r="AF16" s="72" t="str">
+      <c r="Z16" s="72" t="str">
         <f>'Tube O'!G14</f>
         <v>H8</v>
       </c>
-      <c r="AG16" s="73">
+      <c r="AA16" s="73">
         <f>'Tube O'!F14</f>
         <v>1.6974169809999999</v>
       </c>
-      <c r="AH16" s="74">
+      <c r="AB16" s="74">
         <v>4.1784099521668319</v>
       </c>
-      <c r="AI16" s="72" t="str">
+      <c r="AC16" s="72" t="str">
         <f>'Tube P'!G14</f>
         <v>B10</v>
       </c>
-      <c r="AJ16" s="73">
+      <c r="AD16" s="73">
         <f>'Tube P'!F14</f>
         <v>1.7030720140000017</v>
       </c>
-      <c r="AK16" s="76">
+      <c r="AE16" s="76">
         <v>5.942441010764397</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:31">
       <c r="A17" s="56">
         <v>14</v>
       </c>
@@ -21800,94 +20800,72 @@
         <v>1.2962606413750557</v>
       </c>
       <c r="N17" s="72" t="str">
-        <f>'Tube E'!G15</f>
-        <v>C2</v>
-      </c>
-      <c r="O17" s="73">
-        <f>'Tube E'!F15</f>
-        <v>1.6932644929999991</v>
-      </c>
-      <c r="P17" s="75">
-        <v>1.3562277425787963</v>
-      </c>
-      <c r="Q17" s="72" t="str">
-        <f>'Tube F'!G15</f>
-        <v>D5</v>
-      </c>
-      <c r="R17" s="73">
-        <f>'Tube F'!F15</f>
-        <v>1.6918439049999989</v>
-      </c>
-      <c r="S17" s="74">
-        <v>1.6301457107211246</v>
-      </c>
-      <c r="T17" s="72" t="str">
         <f>'Tube G'!G15</f>
         <v>G8</v>
       </c>
-      <c r="U17" s="73">
+      <c r="O17" s="73">
         <f>'Tube G'!F15</f>
         <v>1.6926088369999999</v>
       </c>
-      <c r="V17" s="74">
+      <c r="P17" s="74">
         <v>1.1658049739109311</v>
       </c>
-      <c r="W17" s="72" t="str">
+      <c r="Q17" s="72" t="str">
         <f>'Tube H'!G15</f>
         <v>A10</v>
       </c>
-      <c r="X17" s="73">
+      <c r="R17" s="73">
         <f>'Tube H'!F15</f>
         <v>1.6920897759999995</v>
       </c>
-      <c r="Y17" s="74">
+      <c r="S17" s="74">
         <v>1.6668998085147069</v>
       </c>
-      <c r="Z17" s="72" t="str">
+      <c r="T17" s="72" t="str">
         <f>'Tube M'!G15</f>
         <v>C2</v>
       </c>
-      <c r="AA17" s="73">
+      <c r="U17" s="73">
         <f>'Tube M'!F15</f>
         <v>1.6986463360000013</v>
       </c>
-      <c r="AB17" s="74">
+      <c r="V17" s="74">
         <v>2.3498129555369558</v>
       </c>
-      <c r="AC17" s="72" t="str">
+      <c r="W17" s="72" t="str">
         <f>'Tube N'!G15</f>
         <v>D5</v>
       </c>
-      <c r="AD17" s="73">
+      <c r="X17" s="73">
         <f>'Tube N'!F15</f>
         <v>1.6981272749999992</v>
       </c>
-      <c r="AE17" s="74">
+      <c r="Y17" s="74">
         <v>1.5845553041505323</v>
       </c>
-      <c r="AF17" s="111" t="str">
+      <c r="Z17" s="111" t="str">
         <f>'Tube O'!G15</f>
         <v>G8</v>
       </c>
-      <c r="AG17" s="112">
+      <c r="AA17" s="112">
         <v>1.6876</v>
       </c>
-      <c r="AH17" s="113">
+      <c r="AB17" s="113">
         <v>0</v>
       </c>
-      <c r="AI17" s="72" t="str">
+      <c r="AC17" s="72" t="str">
         <f>'Tube P'!G15</f>
         <v>A10</v>
       </c>
-      <c r="AJ17" s="73">
+      <c r="AD17" s="73">
         <f>'Tube P'!F15</f>
         <v>1.6976082140000006</v>
       </c>
-      <c r="AK17" s="74">
+      <c r="AE17" s="74">
         <v>2.4639658915061049</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:31">
       <c r="A18" s="56">
         <v>15</v>
       </c>
@@ -21936,95 +20914,73 @@
         <v>0.85869842784610206</v>
       </c>
       <c r="N18" s="72" t="str">
-        <f>'Tube E'!G16</f>
-        <v>B2</v>
-      </c>
-      <c r="O18" s="73">
-        <f>'Tube E'!F16</f>
-        <v>1.6878006929999998</v>
-      </c>
-      <c r="P18" s="75">
-        <v>0.83852948806109751</v>
-      </c>
-      <c r="Q18" s="72" t="str">
-        <f>'Tube F'!G16</f>
-        <v>E5</v>
-      </c>
-      <c r="R18" s="73">
-        <f>'Tube F'!F16</f>
-        <v>1.6863801049999996</v>
-      </c>
-      <c r="S18" s="74">
-        <v>0.91438975316711246</v>
-      </c>
-      <c r="T18" s="72" t="str">
         <f>'Tube G'!G16</f>
         <v>F8</v>
       </c>
-      <c r="U18" s="73">
+      <c r="O18" s="73">
         <f>'Tube G'!F16</f>
         <v>1.6860522769999999</v>
       </c>
-      <c r="V18" s="74">
+      <c r="P18" s="74">
         <v>1.1128268040574072</v>
       </c>
-      <c r="W18" s="72" t="str">
+      <c r="Q18" s="72" t="str">
         <f>'Tube H'!G16</f>
         <v>A11</v>
       </c>
-      <c r="X18" s="73">
+      <c r="R18" s="73">
         <f>'Tube H'!F16</f>
         <v>1.6877187360000008</v>
       </c>
-      <c r="Y18" s="74">
+      <c r="S18" s="74">
         <v>1.1722350020350139</v>
       </c>
-      <c r="Z18" s="72" t="str">
+      <c r="T18" s="72" t="str">
         <f>'Tube M'!G16</f>
         <v>B2</v>
       </c>
-      <c r="AA18" s="73">
+      <c r="U18" s="73">
         <f>'Tube M'!F16</f>
         <v>1.6933737690000008</v>
       </c>
-      <c r="AB18" s="74">
+      <c r="V18" s="74">
         <v>1.3798496749477529</v>
       </c>
-      <c r="AC18" s="72" t="str">
+      <c r="W18" s="72" t="str">
         <f>'Tube N'!G16</f>
         <v>E5</v>
       </c>
-      <c r="AD18" s="73">
+      <c r="X18" s="73">
         <f>'Tube N'!F16</f>
         <v>1.6926634749999998</v>
       </c>
-      <c r="AE18" s="74">
+      <c r="Y18" s="74">
         <v>0.98504193888390212</v>
       </c>
-      <c r="AF18" s="72" t="str">
+      <c r="Z18" s="72" t="str">
         <f>'Tube O'!G16</f>
         <v>F8</v>
       </c>
-      <c r="AG18" s="73">
+      <c r="AA18" s="73">
         <f>'Tube O'!F16</f>
         <v>1.6897676610000012</v>
       </c>
-      <c r="AH18" s="74">
+      <c r="AB18" s="74">
         <v>0.8176633527123518</v>
       </c>
-      <c r="AI18" s="72" t="str">
+      <c r="AC18" s="72" t="str">
         <f>'Tube P'!G16</f>
         <v>A11</v>
       </c>
-      <c r="AJ18" s="73">
+      <c r="AD18" s="73">
         <f>'Tube P'!F16</f>
         <v>1.6923356470000002</v>
       </c>
-      <c r="AK18" s="74">
+      <c r="AE18" s="74">
         <v>1.4229340817683054</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:31">
       <c r="A19" s="56">
         <v>16</v>
       </c>
@@ -22073,95 +21029,73 @@
         <v>0.43108788266417225</v>
       </c>
       <c r="N19" s="72" t="str">
-        <f>'Tube E'!G17</f>
-        <v>A2</v>
-      </c>
-      <c r="O19" s="73">
-        <f>'Tube E'!F17</f>
-        <v>1.683429653000001</v>
-      </c>
-      <c r="P19" s="75">
-        <v>0.52749612099034315</v>
-      </c>
-      <c r="Q19" s="72" t="str">
-        <f>'Tube F'!G17</f>
-        <v>F5</v>
-      </c>
-      <c r="R19" s="73">
-        <f>'Tube F'!F17</f>
-        <v>1.6798235450000014</v>
-      </c>
-      <c r="S19" s="74">
-        <v>0.63684669774874458</v>
-      </c>
-      <c r="T19" s="72" t="str">
         <f>'Tube G'!G17</f>
         <v>E8</v>
       </c>
-      <c r="U19" s="73">
+      <c r="O19" s="73">
         <f>'Tube G'!F17</f>
         <v>1.6805884770000006</v>
       </c>
-      <c r="V19" s="74">
+      <c r="P19" s="74">
         <v>0.48272658833967985</v>
       </c>
-      <c r="W19" s="72" t="str">
+      <c r="Q19" s="72" t="str">
         <f>'Tube H'!G17</f>
         <v>B11</v>
       </c>
-      <c r="X19" s="73">
+      <c r="R19" s="73">
         <f>'Tube H'!F17</f>
         <v>1.6811621760000008</v>
       </c>
-      <c r="Y19" s="74">
+      <c r="S19" s="74">
         <v>0.65650037123294924</v>
       </c>
-      <c r="Z19" s="72" t="str">
+      <c r="T19" s="72" t="str">
         <f>'Tube M'!G17</f>
         <v>A2</v>
       </c>
-      <c r="AA19" s="73">
+      <c r="U19" s="73">
         <f>'Tube M'!F17</f>
         <v>1.6879099689999997</v>
       </c>
-      <c r="AB19" s="74">
+      <c r="V19" s="74">
         <v>0.76568008941625665</v>
       </c>
-      <c r="AC19" s="72" t="str">
+      <c r="W19" s="72" t="str">
         <f>'Tube N'!G17</f>
         <v>F5</v>
       </c>
-      <c r="AD19" s="73">
+      <c r="X19" s="73">
         <f>'Tube N'!F17</f>
         <v>1.6861069150000016</v>
       </c>
-      <c r="AE19" s="74">
+      <c r="Y19" s="74">
         <v>0.54133783878258568</v>
       </c>
-      <c r="AF19" s="72" t="str">
+      <c r="Z19" s="72" t="str">
         <f>'Tube O'!G17</f>
         <v>E8</v>
       </c>
-      <c r="AG19" s="73">
+      <c r="AA19" s="73">
         <f>'Tube O'!F17</f>
         <v>1.6832111010000013</v>
       </c>
-      <c r="AH19" s="74">
+      <c r="AB19" s="74">
         <v>0.471490957794509</v>
       </c>
-      <c r="AI19" s="72" t="str">
+      <c r="AC19" s="72" t="str">
         <f>'Tube P'!G17</f>
         <v>B11</v>
       </c>
-      <c r="AJ19" s="73">
+      <c r="AD19" s="73">
         <f>'Tube P'!F17</f>
         <v>1.6868718470000008</v>
       </c>
-      <c r="AK19" s="74">
+      <c r="AE19" s="74">
         <v>0.6259825331673764</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:31">
       <c r="A20" s="56">
         <v>17</v>
       </c>
@@ -22210,95 +21144,73 @@
         <v>0.25607189082030507</v>
       </c>
       <c r="N20" s="72" t="str">
-        <f>'Tube E'!G18</f>
-        <v>A3</v>
-      </c>
-      <c r="O20" s="73">
-        <f>'Tube E'!F18</f>
-        <v>1.6779658530000017</v>
-      </c>
-      <c r="P20" s="74">
-        <v>0.27668119896078913</v>
-      </c>
-      <c r="Q20" s="72" t="str">
-        <f>'Tube F'!G18</f>
-        <v>G5</v>
-      </c>
-      <c r="R20" s="73">
-        <f>'Tube F'!F18</f>
-        <v>1.6754525050000009</v>
-      </c>
-      <c r="S20" s="74">
-        <v>0.38816203621431278</v>
-      </c>
-      <c r="T20" s="72" t="str">
         <f>'Tube G'!G18</f>
         <v>D8</v>
       </c>
-      <c r="U20" s="73">
+      <c r="O20" s="73">
         <f>'Tube G'!F18</f>
         <v>1.6751246770000012</v>
       </c>
-      <c r="V20" s="74">
+      <c r="P20" s="74">
         <v>0.31327492264885731</v>
       </c>
-      <c r="W20" s="72" t="str">
+      <c r="Q20" s="72" t="str">
         <f>'Tube H'!G18</f>
         <v>C11</v>
       </c>
-      <c r="X20" s="73">
+      <c r="R20" s="73">
         <f>'Tube H'!F18</f>
         <v>1.6767911360000021</v>
       </c>
-      <c r="Y20" s="74">
+      <c r="S20" s="74">
         <v>0.38046691109525588</v>
       </c>
-      <c r="Z20" s="72" t="str">
+      <c r="T20" s="72" t="str">
         <f>'Tube M'!G18</f>
         <v>A3</v>
       </c>
-      <c r="AA20" s="73">
+      <c r="U20" s="73">
         <f>'Tube M'!F18</f>
         <v>1.6824461690000003</v>
       </c>
-      <c r="AB20" s="74">
+      <c r="V20" s="74">
         <v>0.40776082336894204</v>
       </c>
-      <c r="AC20" s="72" t="str">
+      <c r="W20" s="72" t="str">
         <f>'Tube N'!G18</f>
         <v>G5</v>
       </c>
-      <c r="AD20" s="73">
+      <c r="X20" s="73">
         <f>'Tube N'!F18</f>
         <v>1.6806431150000023</v>
       </c>
-      <c r="AE20" s="74">
+      <c r="Y20" s="74">
         <v>0.28401286038670026</v>
       </c>
-      <c r="AF20" s="72" t="str">
+      <c r="Z20" s="72" t="str">
         <f>'Tube O'!G18</f>
         <v>D8</v>
       </c>
-      <c r="AG20" s="73">
+      <c r="AA20" s="73">
         <f>'Tube O'!F18</f>
         <v>1.6777473010000019</v>
       </c>
-      <c r="AH20" s="74">
+      <c r="AB20" s="74">
         <v>0.31465127627054207</v>
       </c>
-      <c r="AI20" s="72" t="str">
+      <c r="AC20" s="72" t="str">
         <f>'Tube P'!G18</f>
         <v>C11</v>
       </c>
-      <c r="AJ20" s="73">
+      <c r="AD20" s="73">
         <f>'Tube P'!F18</f>
         <v>1.6803152870000009</v>
       </c>
-      <c r="AK20" s="74">
+      <c r="AE20" s="74">
         <v>0.36225956363776451</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:31">
       <c r="A21" s="56">
         <v>18</v>
       </c>
@@ -22347,95 +21259,73 @@
         <v>0.24272103530632452</v>
       </c>
       <c r="N21" s="72" t="str">
-        <f>'Tube E'!G19</f>
-        <v>B3</v>
-      </c>
-      <c r="O21" s="73">
-        <f>'Tube E'!F19</f>
-        <v>1.671409293</v>
-      </c>
-      <c r="P21" s="74">
-        <v>0.17970421821209173</v>
-      </c>
-      <c r="Q21" s="72" t="str">
-        <f>'Tube F'!G19</f>
-        <v>H5</v>
-      </c>
-      <c r="R21" s="73">
-        <f>'Tube F'!F19</f>
-        <v>1.6678031850000004</v>
-      </c>
-      <c r="S21" s="74">
-        <v>0.30424702451426316</v>
-      </c>
-      <c r="T21" s="72" t="str">
         <f>'Tube G'!G19</f>
         <v>C8</v>
       </c>
-      <c r="U21" s="73">
+      <c r="O21" s="73">
         <f>'Tube G'!F19</f>
         <v>1.6676665899999996</v>
       </c>
-      <c r="V21" s="74">
+      <c r="P21" s="74">
         <v>0.36239751347270405</v>
       </c>
-      <c r="W21" s="72" t="str">
+      <c r="Q21" s="72" t="str">
         <f>'Tube H'!G19</f>
         <v>D11</v>
       </c>
-      <c r="X21" s="73">
+      <c r="R21" s="73">
         <f>'Tube H'!F19</f>
         <v>1.6693330490000005</v>
       </c>
-      <c r="Y21" s="74">
+      <c r="S21" s="74">
         <v>0.34377385774461211</v>
       </c>
-      <c r="Z21" s="72" t="str">
+      <c r="T21" s="72" t="str">
         <f>'Tube M'!G19</f>
         <v>B3</v>
       </c>
-      <c r="AA21" s="73">
+      <c r="U21" s="73">
         <f>'Tube M'!F19</f>
         <v>1.6758896090000022</v>
       </c>
-      <c r="AB21" s="74">
+      <c r="V21" s="74">
         <v>0.29276000123877305</v>
       </c>
-      <c r="AC21" s="72" t="str">
+      <c r="W21" s="72" t="str">
         <f>'Tube N'!G19</f>
         <v>H5</v>
       </c>
-      <c r="AD21" s="73">
+      <c r="X21" s="73">
         <f>'Tube N'!F19</f>
         <v>1.672993795</v>
       </c>
-      <c r="AE21" s="74">
+      <c r="Y21" s="74">
         <v>0.22507097188323297</v>
       </c>
-      <c r="AF21" s="72" t="str">
+      <c r="Z21" s="72" t="str">
         <f>'Tube O'!G19</f>
         <v>C8</v>
       </c>
-      <c r="AG21" s="73">
+      <c r="AA21" s="73">
         <f>'Tube O'!F19</f>
         <v>1.6679124610000002</v>
       </c>
-      <c r="AH21" s="74">
+      <c r="AB21" s="74">
         <v>0.30853803725471635</v>
       </c>
-      <c r="AI21" s="72" t="str">
+      <c r="AC21" s="72" t="str">
         <f>'Tube P'!G19</f>
         <v>D11</v>
       </c>
-      <c r="AJ21" s="73">
+      <c r="AD21" s="73">
         <f>'Tube P'!F19</f>
         <v>1.6737587269999992</v>
       </c>
-      <c r="AK21" s="74">
+      <c r="AE21" s="74">
         <v>0.30441268479843542</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:31">
       <c r="A22" s="56">
         <v>19</v>
       </c>
@@ -22484,95 +21374,73 @@
         <v>0.27509207621942178</v>
       </c>
       <c r="N22" s="72" t="str">
-        <f>'Tube E'!G20</f>
-        <v>C3</v>
-      </c>
-      <c r="O22" s="73">
-        <f>'Tube E'!F20</f>
-        <v>1.6473685729999996</v>
-      </c>
-      <c r="P22" s="74">
-        <v>0.17085276786947276</v>
-      </c>
-      <c r="Q22" s="72" t="str">
-        <f>'Tube F'!G20</f>
-        <v>H6</v>
-      </c>
-      <c r="R22" s="73">
-        <f>'Tube F'!F20</f>
-        <v>1.6483247379999995</v>
-      </c>
-      <c r="S22" s="74">
-        <v>0.33403759007293782</v>
-      </c>
-      <c r="T22" s="72" t="str">
         <f>'Tube G'!G20</f>
         <v>B8</v>
       </c>
-      <c r="U22" s="73">
+      <c r="O22" s="73">
         <f>'Tube G'!F20</f>
         <v>1.6414403499999999</v>
       </c>
-      <c r="V22" s="74">
+      <c r="P22" s="74">
         <v>0.29573581491759127</v>
       </c>
-      <c r="W22" s="72" t="str">
+      <c r="Q22" s="72" t="str">
         <f>'Tube H'!G20</f>
         <v>E11</v>
       </c>
-      <c r="X22" s="73">
+      <c r="R22" s="73">
         <f>'Tube H'!F20</f>
         <v>1.6485706090000001</v>
       </c>
-      <c r="Y22" s="74">
+      <c r="S22" s="74">
         <v>0.37279096058593852</v>
       </c>
-      <c r="Z22" s="72" t="str">
+      <c r="T22" s="72" t="str">
         <f>'Tube M'!G20</f>
         <v>C3</v>
       </c>
-      <c r="AA22" s="73">
+      <c r="U22" s="73">
         <f>'Tube M'!F20</f>
         <v>1.6594982090000006</v>
       </c>
-      <c r="AB22" s="74">
+      <c r="V22" s="74">
         <v>0.28464394883330324</v>
       </c>
-      <c r="AC22" s="72" t="str">
+      <c r="W22" s="72" t="str">
         <f>'Tube N'!G20</f>
         <v>H6</v>
       </c>
-      <c r="AD22" s="73">
+      <c r="X22" s="73">
         <f>'Tube N'!F20</f>
         <v>1.6489530749999997</v>
       </c>
-      <c r="AE22" s="74">
+      <c r="Y22" s="74">
         <v>0.30684574816920362</v>
       </c>
-      <c r="AF22" s="72" t="str">
+      <c r="Z22" s="72" t="str">
         <f>'Tube O'!G20</f>
         <v>B8</v>
       </c>
-      <c r="AG22" s="73">
+      <c r="AA22" s="73">
         <f>'Tube O'!F20</f>
         <v>1.6220165410000007</v>
       </c>
-      <c r="AH22" s="74">
+      <c r="AB22" s="74">
         <v>0.33503877461376219</v>
       </c>
-      <c r="AI22" s="72" t="str">
+      <c r="AC22" s="72" t="str">
         <f>'Tube P'!G20</f>
         <v>E11</v>
       </c>
-      <c r="AJ22" s="73">
+      <c r="AD22" s="73">
         <f>'Tube P'!F20</f>
         <v>1.6529962870000006</v>
       </c>
-      <c r="AK22" s="74">
+      <c r="AE22" s="74">
         <v>0.37039832998299582</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:31">
       <c r="A23" s="56">
         <v>20</v>
       </c>
@@ -22621,95 +21489,73 @@
         <v>0.14689832481370788</v>
       </c>
       <c r="N23" s="72" t="str">
-        <f>'Tube E'!G21</f>
-        <v>D3</v>
-      </c>
-      <c r="O23" s="73">
-        <f>'Tube E'!F21</f>
-        <v>1.5503041660000001</v>
-      </c>
-      <c r="P23" s="74">
-        <v>0.11322053679330339</v>
-      </c>
-      <c r="Q23" s="72" t="str">
-        <f>'Tube F'!G21</f>
-        <v>G6</v>
-      </c>
-      <c r="R23" s="73">
-        <f>'Tube F'!F21</f>
-        <v>1.5456052980000017</v>
-      </c>
-      <c r="S23" s="74">
-        <v>0.24513757490331053</v>
-      </c>
-      <c r="T23" s="72" t="str">
         <f>'Tube G'!G21</f>
         <v>A8</v>
       </c>
-      <c r="U23" s="73">
+      <c r="O23" s="73">
         <f>'Tube G'!F21</f>
         <v>1.5343498699999998</v>
       </c>
-      <c r="V23" s="74">
+      <c r="P23" s="74">
         <v>0.22623885588231551</v>
       </c>
-      <c r="W23" s="72" t="str">
+      <c r="Q23" s="72" t="str">
         <f>'Tube H'!G21</f>
         <v>F11</v>
       </c>
-      <c r="X23" s="73">
+      <c r="R23" s="73">
         <f>'Tube H'!F21</f>
         <v>1.5556860090000004</v>
       </c>
-      <c r="Y23" s="74">
+      <c r="S23" s="74">
         <v>0.24361587357315337</v>
       </c>
-      <c r="Z23" s="72" t="str">
+      <c r="T23" s="72" t="str">
         <f>'Tube M'!G21</f>
         <v>D3</v>
       </c>
-      <c r="AA23" s="73">
+      <c r="U23" s="73">
         <f>'Tube M'!F21</f>
         <v>1.5808194889999996</v>
       </c>
-      <c r="AB23" s="74">
+      <c r="V23" s="74">
         <v>0.31159665368443235</v>
       </c>
-      <c r="AC23" s="72" t="str">
+      <c r="W23" s="72" t="str">
         <f>'Tube N'!G21</f>
         <v>G6</v>
       </c>
-      <c r="AD23" s="73">
+      <c r="X23" s="73">
         <f>'Tube N'!F21</f>
         <v>1.543146587999999</v>
       </c>
-      <c r="AE23" s="74">
+      <c r="Y23" s="74">
         <v>0.23634801406445116</v>
       </c>
-      <c r="AF23" s="72" t="str">
+      <c r="Z23" s="72" t="str">
         <f>'Tube O'!G21</f>
         <v>A8</v>
       </c>
-      <c r="AG23" s="73">
+      <c r="AA23" s="73">
         <f>'Tube O'!F21</f>
         <v>1.4734011809999998</v>
       </c>
-      <c r="AH23" s="74">
+      <c r="AB23" s="74">
         <v>0.20737937141537097</v>
       </c>
-      <c r="AI23" s="72" t="str">
+      <c r="AC23" s="72" t="str">
         <f>'Tube P'!G21</f>
         <v>F11</v>
       </c>
-      <c r="AJ23" s="73">
+      <c r="AD23" s="73">
         <f>'Tube P'!F21</f>
         <v>1.5590189270000003</v>
       </c>
-      <c r="AK23" s="74">
+      <c r="AE23" s="74">
         <v>0.24272611441916739</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:31">
       <c r="A24" s="56">
         <v>21</v>
       </c>
@@ -22758,95 +21604,73 @@
         <v>9.5493150670842339E-2</v>
       </c>
       <c r="N24" s="69" t="str">
-        <f>'Tube E'!G22</f>
-        <v>E3</v>
-      </c>
-      <c r="O24" s="70">
-        <f>'Tube E'!F22</f>
-        <v>1.3339376860000005</v>
-      </c>
-      <c r="P24" s="71">
-        <v>6.6394910224652201E-2</v>
-      </c>
-      <c r="Q24" s="69" t="str">
-        <f>'Tube F'!G22</f>
-        <v>F6</v>
-      </c>
-      <c r="R24" s="70">
-        <f>'Tube F'!F22</f>
-        <v>1.3270532980000009</v>
-      </c>
-      <c r="S24" s="71">
-        <v>0.13722067463848683</v>
-      </c>
-      <c r="T24" s="69" t="str">
         <f>'Tube G'!G22</f>
         <v>A9</v>
       </c>
-      <c r="U24" s="70">
+      <c r="O24" s="70">
         <f>'Tube G'!F22</f>
         <v>1.3114268300000003</v>
       </c>
-      <c r="V24" s="71">
+      <c r="P24" s="71">
         <v>0.12648154709212375</v>
       </c>
-      <c r="W24" s="69" t="str">
+      <c r="Q24" s="69" t="str">
         <f>'Tube H'!G22</f>
         <v>G11</v>
       </c>
-      <c r="X24" s="70">
+      <c r="R24" s="70">
         <f>'Tube H'!F22</f>
         <v>1.3568036890000013</v>
       </c>
-      <c r="Y24" s="71">
+      <c r="S24" s="71">
         <v>0.15168361080621834</v>
       </c>
-      <c r="Z24" s="69" t="str">
+      <c r="T24" s="69" t="str">
         <f>'Tube M'!G22</f>
         <v>E3</v>
       </c>
-      <c r="AA24" s="70">
+      <c r="U24" s="70">
         <f>'Tube M'!F22</f>
         <v>1.383029929000001</v>
       </c>
-      <c r="AB24" s="71">
+      <c r="V24" s="71">
         <v>0.14171468903984297</v>
       </c>
-      <c r="AC24" s="69" t="str">
+      <c r="W24" s="69" t="str">
         <f>'Tube N'!G22</f>
         <v>F6</v>
       </c>
-      <c r="AD24" s="70">
+      <c r="X24" s="70">
         <f>'Tube N'!F22</f>
         <v>1.3235018279999995</v>
       </c>
-      <c r="AE24" s="71">
+      <c r="Y24" s="71">
         <v>0.12257788451101033</v>
       </c>
-      <c r="AF24" s="69" t="str">
+      <c r="Z24" s="69" t="str">
         <f>'Tube O'!G22</f>
         <v>A9</v>
       </c>
-      <c r="AG24" s="70">
+      <c r="AA24" s="70">
         <f>'Tube O'!F22</f>
         <v>1.2331852140000006</v>
       </c>
-      <c r="AH24" s="71">
+      <c r="AB24" s="71">
         <v>8.2658623408786866E-2</v>
       </c>
-      <c r="AI24" s="69" t="str">
+      <c r="AC24" s="69" t="str">
         <f>'Tube P'!G22</f>
         <v>G11</v>
       </c>
-      <c r="AJ24" s="70">
+      <c r="AD24" s="70">
         <f>'Tube P'!F22</f>
         <v>1.3481162470000019</v>
       </c>
-      <c r="AK24" s="71">
+      <c r="AE24" s="71">
         <v>0.14465994850337924</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="12.9" thickBot="1">
+    <row r="25" spans="1:31" ht="12.9" thickBot="1">
       <c r="A25" s="56">
         <v>22</v>
       </c>
@@ -22894,99 +21718,77 @@
       <c r="M25" s="80">
         <v>5.1375171438548778E-2</v>
       </c>
-      <c r="N25" s="78" t="str">
-        <f>'Tube E'!G23</f>
-        <v>F3</v>
-      </c>
-      <c r="O25" s="79">
-        <f>'Tube E'!F23</f>
-        <v>1.1066436060000004</v>
-      </c>
-      <c r="P25" s="80">
-        <v>1.2021890825825386E-2</v>
-      </c>
-      <c r="Q25" s="78" t="str">
-        <f>'Tube F'!G23</f>
-        <v>E6</v>
-      </c>
-      <c r="R25" s="79">
-        <f>'Tube F'!F23</f>
-        <v>1.1106868180000014</v>
-      </c>
-      <c r="S25" s="80">
-        <v>0.17936213691288194</v>
-      </c>
-      <c r="T25" s="69" t="str">
+      <c r="N25" s="69" t="str">
         <f>'Tube G'!G23</f>
         <v>B9</v>
       </c>
-      <c r="U25" s="79">
+      <c r="O25" s="79">
         <f>'Tube G'!F23</f>
         <v>1.1070807100000017</v>
       </c>
-      <c r="V25" s="80">
+      <c r="P25" s="80">
         <v>4.0870273539470585E-2</v>
       </c>
-      <c r="W25" s="78" t="str">
+      <c r="Q25" s="78" t="str">
         <f>'Tube H'!G23</f>
         <v>H11</v>
       </c>
-      <c r="X25" s="79">
+      <c r="R25" s="79">
         <f>'Tube H'!F23</f>
         <v>1.1338806490000017</v>
       </c>
-      <c r="Y25" s="80">
+      <c r="S25" s="80">
         <v>7.7027221348113198E-2</v>
       </c>
-      <c r="Z25" s="69" t="str">
+      <c r="T25" s="69" t="str">
         <f>'Tube M'!G23</f>
         <v>F3</v>
       </c>
-      <c r="AA25" s="70">
+      <c r="U25" s="70">
         <f>'Tube M'!F23</f>
         <v>1.1404372089999999</v>
       </c>
-      <c r="AB25" s="71">
+      <c r="V25" s="71">
         <v>5.3174064862824409E-2</v>
       </c>
-      <c r="AC25" s="89" t="str">
+      <c r="W25" s="89" t="str">
         <f>'Tube N'!G23</f>
         <v>E6</v>
       </c>
-      <c r="AD25" s="70">
+      <c r="X25" s="70">
         <f>'Tube N'!F23</f>
         <v>1.1224339879999992</v>
       </c>
-      <c r="AE25" s="88">
+      <c r="Y25" s="88">
         <v>3.3613356235393188E-2</v>
       </c>
-      <c r="AF25" s="69" t="str">
+      <c r="Z25" s="69" t="str">
         <f>'Tube O'!G23</f>
         <v>B9</v>
       </c>
-      <c r="AG25" s="70">
+      <c r="AA25" s="70">
         <f>'Tube O'!F23</f>
         <v>1.0954974540000002</v>
       </c>
-      <c r="AH25" s="88">
+      <c r="AB25" s="88">
         <v>2.7534671937592476E-2</v>
       </c>
-      <c r="AI25" s="69" t="str">
+      <c r="AC25" s="69" t="str">
         <f>'Tube P'!G23</f>
         <v>H11</v>
       </c>
-      <c r="AJ25" s="70">
+      <c r="AD25" s="70">
         <f>'Tube P'!F23</f>
         <v>1.1350280470000005</v>
       </c>
-      <c r="AK25" s="80">
+      <c r="AE25" s="80">
         <v>8.0676371015666395E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="12.9" thickTop="1">
+    <row r="26" spans="1:31" ht="12.9" thickTop="1">
       <c r="B26" s="73"/>
       <c r="C26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D26" s="82">
         <f>SUM(D5:D25)*40/TubeLoading!J29*100</f>
@@ -22994,7 +21796,7 @@
       </c>
       <c r="E26" s="73"/>
       <c r="F26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G26" s="82">
         <f>SUM(G5:G25)*40/TubeLoading!J30*100</f>
@@ -23002,7 +21804,7 @@
       </c>
       <c r="H26" s="73"/>
       <c r="I26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J26" s="82">
         <f>SUM(J5:J25)*40/TubeLoading!J31*100</f>
@@ -23010,78 +21812,62 @@
       </c>
       <c r="K26" s="83"/>
       <c r="L26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M26" s="82">
         <f>SUM(M5:M25)*40/TubeLoading!J32*100</f>
         <v>57.622146731846172</v>
       </c>
-      <c r="N26" s="73"/>
+      <c r="N26" s="87"/>
       <c r="O26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P26" s="82">
-        <f>SUM(P5:P25)*40/TubeLoading!J33*100</f>
-        <v>44.543408475176868</v>
+        <f>SUM(P5:P25)*40/TubeLoading!J35*100</f>
+        <v>64.286969553839086</v>
       </c>
       <c r="Q26" s="73"/>
       <c r="R26" s="81" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="S26" s="82">
-        <f>SUM(S5:S25)*40/TubeLoading!J34*100</f>
-        <v>75.593595322285182</v>
-      </c>
-      <c r="T26" s="87"/>
-      <c r="U26" s="81" t="s">
-        <v>190</v>
-      </c>
-      <c r="V26" s="82">
-        <f>SUM(V5:V25)*40/TubeLoading!J35*100</f>
-        <v>64.286969553839086</v>
+        <f>SUM(S5:S25)*40/TubeLoading!J36*100</f>
+        <v>73.330591175662391</v>
+      </c>
+      <c r="T26" s="90"/>
+      <c r="U26" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="V26" s="92">
+        <f>SUM(V5:V25)*40/TubeLoading!J41*100</f>
+        <v>80.45097095349729</v>
       </c>
       <c r="W26" s="73"/>
-      <c r="X26" s="81" t="s">
-        <v>190</v>
+      <c r="X26" s="91" t="s">
+        <v>188</v>
       </c>
       <c r="Y26" s="82">
-        <f>SUM(Y5:Y25)*40/TubeLoading!J36*100</f>
-        <v>73.330591175662391</v>
+        <f>SUM(Y5:Y25)*40/TubeLoading!J42*100</f>
+        <v>73.835192341047971</v>
       </c>
       <c r="Z26" s="90"/>
       <c r="AA26" s="91" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB26" s="92">
-        <f>SUM(AB5:AB25)*40/TubeLoading!J41*100</f>
-        <v>80.45097095349729</v>
-      </c>
-      <c r="AC26" s="73"/>
-      <c r="AD26" s="91" t="s">
-        <v>190</v>
+        <v>188</v>
+      </c>
+      <c r="AB26" s="82">
+        <f>SUM(AB5:AB25)*40/TubeLoading!J43*100</f>
+        <v>66.667936426690574</v>
+      </c>
+      <c r="AC26" s="83"/>
+      <c r="AD26" s="81" t="s">
+        <v>188</v>
       </c>
       <c r="AE26" s="82">
-        <f>SUM(AE5:AE25)*40/TubeLoading!J42*100</f>
-        <v>73.835192341047971</v>
-      </c>
-      <c r="AF26" s="90"/>
-      <c r="AG26" s="91" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH26" s="82">
-        <f>SUM(AH5:AH25)*40/TubeLoading!J43*100</f>
-        <v>66.667936426690574</v>
-      </c>
-      <c r="AI26" s="83"/>
-      <c r="AJ26" s="81" t="s">
-        <v>190</v>
-      </c>
-      <c r="AK26" s="82">
-        <f>SUM(AK5:AK25)*40/TubeLoading!J44*100</f>
+        <f>SUM(AE5:AE25)*40/TubeLoading!J44*100</f>
         <v>71.313343562102091</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:31">
       <c r="B27" s="73"/>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
@@ -23095,7 +21881,7 @@
       <c r="L27" s="73"/>
       <c r="M27" s="73"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:31">
       <c r="B28" s="73"/>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -23109,13 +21895,13 @@
       <c r="L28" s="73"/>
       <c r="M28" s="73"/>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:31">
       <c r="A29" s="62"/>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:31">
       <c r="A30" s="62"/>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:31">
       <c r="A31" s="62"/>
     </row>
     <row r="55" spans="1:13">
@@ -23179,19 +21965,17 @@
       <c r="A86" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Y2"/>
+  <mergeCells count="10">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24053,13 +22837,13 @@
         <v>148</v>
       </c>
       <c r="J28" s="108" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K28" s="109" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L28" s="109" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="14.15">
@@ -24808,7 +23592,7 @@
       <c r="B46" s="26"/>
       <c r="C46" s="23"/>
       <c r="F46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -27125,7 +25909,7 @@
         <v>1.6918985430000006</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -27150,7 +25934,7 @@
         <v>1.6842492230000001</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -27175,7 +25959,7 @@
         <v>1.6787854230000008</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -27200,7 +25984,7 @@
         <v>1.6689505830000009</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -27225,7 +26009,7 @@
         <v>1.6307039830000001</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -27250,7 +26034,7 @@
         <v>1.5161554160000001</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -27275,7 +26059,7 @@
         <v>1.3314789760000014</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -27300,7 +26084,7 @@
         <v>1.1478952960000015</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>